<commit_message>
Add 2 new data for DCEP VStar.
</commit_message>
<xml_diff>
--- a/delta_cep/delta_cep.xlsx
+++ b/delta_cep/delta_cep.xlsx
@@ -17,6 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0_ "/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -56,8 +59,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -114,10 +120,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$1:$D$11</c:f>
+              <c:f>Sheet1!$D$1:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0.76597222222222228</c:v>
                 </c:pt>
@@ -150,16 +156,22 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>11.897916666666667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.88125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.9125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$1:$E$11</c:f>
+              <c:f>Sheet1!$E$1:$E$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:formatCode>0.0_ </c:formatCode>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>3.6</c:v>
                 </c:pt>
@@ -192,6 +204,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -206,11 +224,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="51167232"/>
-        <c:axId val="51168768"/>
+        <c:axId val="41367040"/>
+        <c:axId val="116416512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51167232"/>
+        <c:axId val="41367040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -220,12 +238,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51168768"/>
+        <c:crossAx val="116416512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51168768"/>
+        <c:axId val="116416512"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:min val="3"/>
@@ -233,11 +251,11 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0_ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51167232"/>
+        <c:crossAx val="41367040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -284,10 +302,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$1:$F$11</c:f>
+              <c:f>Sheet1!$F$1:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0.76597222222222228</c:v>
                 </c:pt>
@@ -304,32 +322,38 @@
                   <c:v>4.2004629629629635</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.46263888888888882</c:v>
+                  <c:v>0.46663888888888927</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4723611111111108</c:v>
+                  <c:v>1.4763611111111112</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5522222222222224</c:v>
+                  <c:v>2.5562222222222228</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.4362500000000002</c:v>
+                  <c:v>4.4402500000000007</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.17805555555555586</c:v>
+                  <c:v>0.18605555555555675</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1579166666666669</c:v>
+                  <c:v>1.1659166666666678</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1492500000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.1805000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$1:$E$11</c:f>
+              <c:f>Sheet1!$E$1:$E$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:formatCode>0.0_ </c:formatCode>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>3.6</c:v>
                 </c:pt>
@@ -362,6 +386,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -376,11 +406,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="76489088"/>
-        <c:axId val="76490624"/>
+        <c:axId val="116440064"/>
+        <c:axId val="116441856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76489088"/>
+        <c:axId val="116440064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -390,12 +420,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76490624"/>
+        <c:crossAx val="116441856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76490624"/>
+        <c:axId val="116441856"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:min val="3"/>
@@ -404,11 +434,11 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0_ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76489088"/>
+        <c:crossAx val="116440064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="0.1"/>
@@ -778,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -790,7 +820,7 @@
     <col min="2" max="2" width="7.75" customWidth="1"/>
     <col min="3" max="3" width="4.875" customWidth="1"/>
     <col min="4" max="4" width="10.25" customWidth="1"/>
-    <col min="5" max="5" width="5.25" customWidth="1"/>
+    <col min="5" max="5" width="5.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
@@ -807,7 +837,7 @@
         <f>(A1*1440+B1*60+C1)/1440</f>
         <v>0.76597222222222228</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <v>3.6</v>
       </c>
       <c r="F1">
@@ -829,7 +859,7 @@
         <f t="shared" ref="D2:F11" si="0">(A2*1440+B2*60+C2)/1440</f>
         <v>1.8236111111111111</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>4</v>
       </c>
       <c r="F2">
@@ -851,7 +881,7 @@
         <f t="shared" si="0"/>
         <v>2.9083333333333332</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>4.2</v>
       </c>
       <c r="F3">
@@ -873,7 +903,7 @@
         <f t="shared" si="0"/>
         <v>3.8576388888888888</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>3.4</v>
       </c>
       <c r="F4">
@@ -895,7 +925,7 @@
         <f t="shared" si="0"/>
         <v>4.7527777777777782</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>3.5</v>
       </c>
       <c r="F5">
@@ -917,12 +947,12 @@
         <f t="shared" si="0"/>
         <v>5.8326388888888889</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>3.7</v>
       </c>
       <c r="F6">
-        <f>D6-5.37</f>
-        <v>0.46263888888888882</v>
+        <f>D6-5.366</f>
+        <v>0.46663888888888927</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -939,12 +969,12 @@
         <f t="shared" si="0"/>
         <v>6.8423611111111109</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>4.0999999999999996</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F9" si="2">D7-5.37</f>
-        <v>1.4723611111111108</v>
+        <f t="shared" ref="F7:F9" si="2">D7-5.366</f>
+        <v>1.4763611111111112</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
@@ -961,12 +991,12 @@
         <f t="shared" si="0"/>
         <v>7.9222222222222225</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>4.3</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
-        <v>2.5522222222222224</v>
+        <v>2.5562222222222228</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
@@ -983,12 +1013,12 @@
         <f t="shared" si="0"/>
         <v>9.8062500000000004</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>3.4</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
-        <v>4.4362500000000002</v>
+        <v>4.4402500000000007</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -1005,12 +1035,12 @@
         <f t="shared" si="0"/>
         <v>10.918055555555556</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>3.6</v>
       </c>
       <c r="F10">
-        <f>D10-5.37*2</f>
-        <v>0.17805555555555586</v>
+        <f>D10-5.366*2</f>
+        <v>0.18605555555555675</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
@@ -1027,18 +1057,63 @@
         <f t="shared" si="0"/>
         <v>11.897916666666667</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>3.8</v>
       </c>
       <c r="F11">
-        <f>D11-5.37*2</f>
-        <v>1.1579166666666669</v>
+        <f t="shared" ref="F11:F13" si="3">D11-5.366*2</f>
+        <v>1.1659166666666678</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <f>(A12*1440+B12*60+C12)/1440</f>
+        <v>12.88125</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="3"/>
+        <v>2.1492500000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>54</v>
+      </c>
+      <c r="D13">
+        <f>(A13*1440+B13*60+C13)/1440</f>
+        <v>13.9125</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>3.1805000000000003</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add new observation data
</commit_message>
<xml_diff>
--- a/delta_cep/delta_cep.xlsx
+++ b/delta_cep/delta_cep.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18180" windowHeight="8550"/>
+    <workbookView windowWidth="16980" windowHeight="10935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,36 +16,369 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.0_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -53,24 +386,316 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -94,84 +719,92 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.6224628171478584E-2"/>
-          <c:y val="8.5614312138559287E-2"/>
-          <c:w val="0.87635870516185477"/>
-          <c:h val="0.86572266210456283"/>
+          <c:x val="0.0762246281714786"/>
+          <c:y val="0.0856143121385593"/>
+          <c:w val="0.876358705161855"/>
+          <c:h val="0.865722662104563"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="marker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="28575">
+            <a:ln w="28575" cap="rnd" cmpd="sng" algn="ctr">
               <a:noFill/>
+              <a:prstDash val="solid"/>
+              <a:round/>
             </a:ln>
           </c:spPr>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$1:$D$13</c:f>
+              <c:f>Sheet1!$E$1:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.76597222222222228</c:v>
+                  <c:v>0.765972222222222</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8236111111111111</c:v>
+                  <c:v>1.82361111111111</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9083333333333332</c:v>
+                  <c:v>2.90833333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8576388888888888</c:v>
+                  <c:v>3.85763888888889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.7527777777777782</c:v>
+                  <c:v>4.75277777777778</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.8326388888888889</c:v>
+                  <c:v>5.83263888888889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.8423611111111109</c:v>
+                  <c:v>6.84236111111111</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.9222222222222225</c:v>
+                  <c:v>7.92222222222222</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.8062500000000004</c:v>
+                  <c:v>9.80625</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.918055555555556</c:v>
+                  <c:v>10.9180555555556</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.897916666666667</c:v>
+                  <c:v>11.8979166666667</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12.88125</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>13.9125</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16.7548611111111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$1:$E$13</c:f>
+              <c:f>Sheet1!$F$1:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>3.6</c:v>
                 </c:pt>
@@ -191,7 +824,7 @@
                   <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0999999999999996</c:v>
+                  <c:v>4.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>4.3</c:v>
@@ -210,6 +843,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -238,6 +874,22 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="116416512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -255,6 +907,22 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="41367040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -264,6 +932,15 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="zh-CN"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -286,74 +963,82 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="marker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="28575">
+            <a:ln w="28575" cap="rnd" cmpd="sng" algn="ctr">
               <a:noFill/>
+              <a:prstDash val="solid"/>
+              <a:round/>
             </a:ln>
           </c:spPr>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$1:$F$13</c:f>
+              <c:f>Sheet1!$G$1:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.76597222222222228</c:v>
+                  <c:v>0.765972222222222</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8236111111111111</c:v>
+                  <c:v>1.82361111111111</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9083333333333332</c:v>
+                  <c:v>2.90833333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8576388888888888</c:v>
+                  <c:v>3.85763888888889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.2004629629629635</c:v>
+                  <c:v>4.20046296296296</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.46663888888888927</c:v>
+                  <c:v>0.466638888888889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4763611111111112</c:v>
+                  <c:v>1.47636111111111</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5562222222222228</c:v>
+                  <c:v>2.55622222222222</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.4402500000000007</c:v>
+                  <c:v>4.44025</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.18605555555555675</c:v>
+                  <c:v>0.186055555555557</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1659166666666678</c:v>
+                  <c:v>1.16591666666667</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.1492500000000003</c:v>
+                  <c:v>2.14925</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.1805000000000003</c:v>
+                  <c:v>3.1805</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.656861111111112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$1:$E$13</c:f>
+              <c:f>Sheet1!$F$1:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>3.6</c:v>
                 </c:pt>
@@ -373,7 +1058,7 @@
                   <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0999999999999996</c:v>
+                  <c:v>4.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>4.3</c:v>
@@ -392,6 +1077,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -420,6 +1108,22 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="116441856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -438,6 +1142,22 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="116440064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -448,6 +1168,15 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="zh-CN"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -457,28 +1186,28 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>152399</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>142874</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="4361815" y="152400"/>
+        <a:ext cx="4791075" cy="3419475"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -490,25 +1219,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="图表 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="9429750" y="161925"/>
+        <a:ext cx="3009900" cy="3600450"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -802,343 +1531,415 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="5.375" customWidth="1"/>
-    <col min="2" max="2" width="7.75" customWidth="1"/>
-    <col min="3" max="3" width="4.875" customWidth="1"/>
-    <col min="4" max="4" width="10.25" customWidth="1"/>
-    <col min="5" max="5" width="5.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125"/>
+    <col min="2" max="2" width="5.375" customWidth="1"/>
+    <col min="3" max="3" width="7.75" customWidth="1"/>
+    <col min="4" max="4" width="4.875" customWidth="1"/>
+    <col min="5" max="5" width="10.25" customWidth="1"/>
+    <col min="6" max="6" width="5.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A1">
+    <row r="1" spans="1:7">
+      <c r="A1" s="2">
+        <v>43028</v>
+      </c>
+      <c r="B1">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="C1">
         <v>18</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>23</v>
       </c>
-      <c r="D1">
-        <f>(A1*1440+B1*60+C1)/1440</f>
-        <v>0.76597222222222228</v>
-      </c>
-      <c r="E1" s="1">
+      <c r="E1">
+        <f>(B1*1440+C1*60+D1)/1440</f>
+        <v>0.765972222222222</v>
+      </c>
+      <c r="F1" s="1">
         <v>3.6</v>
       </c>
-      <c r="F1">
-        <f>D1</f>
-        <v>0.76597222222222228</v>
+      <c r="G1">
+        <f>E1</f>
+        <v>0.765972222222222</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2">
+    <row r="2" spans="1:7">
+      <c r="A2" s="2">
+        <v>43029</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>19</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>46</v>
       </c>
-      <c r="D2">
-        <f t="shared" ref="D2:F11" si="0">(A2*1440+B2*60+C2)/1440</f>
-        <v>1.8236111111111111</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="E2">
+        <f t="shared" ref="E2:G11" si="0">(B2*1440+C2*60+D2)/1440</f>
+        <v>1.82361111111111</v>
+      </c>
+      <c r="F2" s="1">
         <v>4</v>
       </c>
-      <c r="F2">
-        <f t="shared" ref="F2:F4" si="1">D2</f>
-        <v>1.8236111111111111</v>
+      <c r="G2">
+        <f t="shared" ref="G2:G4" si="1">E2</f>
+        <v>1.82361111111111</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3">
+    <row r="3" spans="1:7">
+      <c r="A3" s="2">
+        <v>43030</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>21</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>48</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <f t="shared" si="0"/>
-        <v>2.9083333333333332</v>
-      </c>
-      <c r="E3" s="1">
+        <v>2.90833333333333</v>
+      </c>
+      <c r="F3" s="1">
         <v>4.2</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <f t="shared" si="1"/>
-        <v>2.9083333333333332</v>
+        <v>2.90833333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4">
+    <row r="4" spans="1:7">
+      <c r="A4" s="2">
+        <v>43031</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>20</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>35</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <f t="shared" si="0"/>
-        <v>3.8576388888888888</v>
-      </c>
-      <c r="E4" s="1">
+        <v>3.85763888888889</v>
+      </c>
+      <c r="F4" s="1">
         <v>3.4</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <f t="shared" si="1"/>
-        <v>3.8576388888888888</v>
+        <v>3.85763888888889</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5">
+    <row r="5" spans="1:7">
+      <c r="A5" s="2">
+        <v>43032</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>18</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f t="shared" si="0"/>
-        <v>4.7527777777777782</v>
-      </c>
-      <c r="E5" s="1">
+        <v>4.75277777777778</v>
+      </c>
+      <c r="F5" s="1">
         <v>3.5</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <f t="shared" si="0"/>
-        <v>4.2004629629629635</v>
+        <v>4.20046296296296</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6">
+    <row r="6" spans="1:7">
+      <c r="A6" s="2">
+        <v>43033</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>19</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>59</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f t="shared" si="0"/>
-        <v>5.8326388888888889</v>
-      </c>
-      <c r="E6" s="1">
+        <v>5.83263888888889</v>
+      </c>
+      <c r="F6" s="1">
         <v>3.7</v>
       </c>
-      <c r="F6">
-        <f>D6-5.366</f>
-        <v>0.46663888888888927</v>
+      <c r="G6">
+        <f>E6-5.366</f>
+        <v>0.466638888888889</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7">
+    <row r="7" spans="1:7">
+      <c r="A7" s="2">
+        <v>43034</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>20</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>13</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <f t="shared" si="0"/>
-        <v>6.8423611111111109</v>
-      </c>
-      <c r="E7" s="1">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F7">
-        <f t="shared" ref="F7:F9" si="2">D7-5.366</f>
-        <v>1.4763611111111112</v>
+        <v>6.84236111111111</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4.1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G9" si="2">E7-5.366</f>
+        <v>1.47636111111111</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8">
+    <row r="8" spans="1:7">
+      <c r="A8" s="2">
+        <v>43035</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>22</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>8</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <f t="shared" si="0"/>
-        <v>7.9222222222222225</v>
-      </c>
-      <c r="E8" s="1">
+        <v>7.92222222222222</v>
+      </c>
+      <c r="F8" s="1">
         <v>4.3</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <f t="shared" si="2"/>
-        <v>2.5562222222222228</v>
+        <v>2.55622222222222</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9">
+    <row r="9" spans="1:7">
+      <c r="A9" s="2">
+        <v>43037</v>
+      </c>
+      <c r="B9">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>19</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>21</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <f t="shared" si="0"/>
-        <v>9.8062500000000004</v>
-      </c>
-      <c r="E9" s="1">
+        <v>9.80625</v>
+      </c>
+      <c r="F9" s="1">
         <v>3.4</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <f t="shared" si="2"/>
-        <v>4.4402500000000007</v>
+        <v>4.44025</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10">
+    <row r="10" spans="1:7">
+      <c r="A10" s="2">
+        <v>43038</v>
+      </c>
+      <c r="B10">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>22</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>2</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <f t="shared" si="0"/>
-        <v>10.918055555555556</v>
-      </c>
-      <c r="E10" s="1">
+        <v>10.9180555555556</v>
+      </c>
+      <c r="F10" s="1">
         <v>3.6</v>
       </c>
-      <c r="F10">
-        <f>D10-5.366*2</f>
-        <v>0.18605555555555675</v>
+      <c r="G10">
+        <f>E10-5.366*2</f>
+        <v>0.186055555555557</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11">
+    <row r="11" spans="1:7">
+      <c r="A11" s="2">
+        <v>43039</v>
+      </c>
+      <c r="B11">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>21</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>33</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <f t="shared" si="0"/>
-        <v>11.897916666666667</v>
-      </c>
-      <c r="E11" s="1">
+        <v>11.8979166666667</v>
+      </c>
+      <c r="F11" s="1">
         <v>3.8</v>
       </c>
-      <c r="F11">
-        <f t="shared" ref="F11:F13" si="3">D11-5.366*2</f>
-        <v>1.1659166666666678</v>
+      <c r="G11">
+        <f t="shared" ref="G11:G14" si="3">E11-5.366*2</f>
+        <v>1.16591666666667</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12">
+    <row r="12" spans="1:7">
+      <c r="A12" s="2">
+        <v>43040</v>
+      </c>
+      <c r="B12">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>21</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>9</v>
       </c>
-      <c r="D12">
-        <f>(A12*1440+B12*60+C12)/1440</f>
+      <c r="E12">
+        <f t="shared" ref="E12:E14" si="4">(B12*1440+C12*60+D12)/1440</f>
         <v>12.88125</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>4</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <f t="shared" si="3"/>
-        <v>2.1492500000000003</v>
+        <v>2.14925</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13">
+    <row r="13" spans="1:7">
+      <c r="A13" s="2">
+        <v>43041</v>
+      </c>
+      <c r="B13">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>21</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>54</v>
       </c>
-      <c r="D13">
-        <f>(A13*1440+B13*60+C13)/1440</f>
+      <c r="E13">
+        <f t="shared" si="4"/>
         <v>13.9125</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>3.7</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <f t="shared" si="3"/>
-        <v>3.1805000000000003</v>
+        <v>3.1805</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2">
+        <v>43044</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>18</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="4"/>
+        <v>16.7548611111111</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G14">
+        <f>E14-5.366*3</f>
+        <v>0.656861111111112</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add data in two days.
</commit_message>
<xml_diff>
--- a/delta_cep/delta_cep.xlsx
+++ b/delta_cep/delta_cep.xlsx
@@ -18,15 +18,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="0.0_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.0_ "/>
   </numFmts>
   <fonts count="21">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -42,55 +49,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -102,54 +63,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,8 +90,87 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -193,187 +193,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,6 +384,54 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -398,6 +446,17 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -425,212 +484,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -750,10 +750,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$1:$E$14</c:f>
+              <c:f>Sheet1!$E$1:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.765972222222222</c:v>
                 </c:pt>
@@ -795,16 +795,22 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>16.7548611111111</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.8326388888889</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.7777777777778</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$1:$F$14</c:f>
+              <c:f>Sheet1!$F$1:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>3.6</c:v>
                 </c:pt>
@@ -845,6 +851,12 @@
                   <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -984,10 +996,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$1:$G$14</c:f>
+              <c:f>Sheet1!$G$1:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.765972222222222</c:v>
                 </c:pt>
@@ -1029,16 +1041,22 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.656861111111112</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.73463888888889</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.67977777777778</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$1:$F$14</c:f>
+              <c:f>Sheet1!$F$1:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>3.6</c:v>
                 </c:pt>
@@ -1079,6 +1097,12 @@
                   <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -1537,10 +1561,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -1843,7 +1867,7 @@
         <v>9</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12:E14" si="4">(B12*1440+C12*60+D12)/1440</f>
+        <f t="shared" ref="E12:E16" si="4">(B12*1440+C12*60+D12)/1440</f>
         <v>12.88125</v>
       </c>
       <c r="F12" s="1">
@@ -1900,8 +1924,58 @@
         <v>3.5</v>
       </c>
       <c r="G14">
-        <f>E14-5.366*3</f>
+        <f t="shared" ref="G14:G16" si="5">E14-5.366*3</f>
         <v>0.656861111111112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="2">
+        <v>43047</v>
+      </c>
+      <c r="B15">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <v>59</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="4"/>
+        <v>19.8326388888889</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>3.73463888888889</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="2">
+        <v>43048</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>18</v>
+      </c>
+      <c r="D16">
+        <v>40</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="4"/>
+        <v>20.7777777777778</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>4.67977777777778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Add data to Delta Cep. 2. Modify Simpson integration to decrease the times of multiple calculations. 3. After update to Ruby 2.4.2, re-compile the C dll.
</commit_message>
<xml_diff>
--- a/delta_cep/delta_cep.xlsx
+++ b/delta_cep/delta_cep.xlsx
@@ -18,11 +18,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.0_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -33,40 +33,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -108,19 +85,47 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -148,24 +153,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -193,6 +193,78 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -223,19 +295,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,72 +338,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,6 +384,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -407,6 +422,26 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -443,41 +478,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -489,148 +489,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -750,10 +750,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$1:$E$19</c:f>
+              <c:f>Sheet1!$E$1:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.765972222222222</c:v>
                 </c:pt>
@@ -810,16 +810,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>26.7854166666667</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>29.9131944444444</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$1:$F$19</c:f>
+              <c:f>Sheet1!$F$1:$F$20</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>3.6</c:v>
                 </c:pt>
@@ -876,6 +879,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1024,10 +1030,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$1:$G$19</c:f>
+              <c:f>Sheet1!$G$1:$G$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.765972222222222</c:v>
                 </c:pt>
@@ -1084,16 +1090,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>5.32141666666667</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.08319444444444</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$1:$F$19</c:f>
+              <c:f>Sheet1!$F$1:$F$20</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>3.6</c:v>
                 </c:pt>
@@ -1150,6 +1159,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1267,8 +1279,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>142240</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>10795</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1277,7 +1289,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4361815" y="152400"/>
-        <a:ext cx="4791075" cy="3629025"/>
+        <a:ext cx="4791075" cy="2773045"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1289,16 +1301,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>685165</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>55880</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1306,8 +1318,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9429750" y="161925"/>
-        <a:ext cx="3695065" cy="3600450"/>
+        <a:off x="4371975" y="2971800"/>
+        <a:ext cx="4694555" cy="3257550"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1607,10 +1619,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -1913,7 +1925,7 @@
         <v>9</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12:E19" si="4">(B12*1440+C12*60+D12)/1440</f>
+        <f t="shared" ref="E12:E20" si="4">(B12*1440+C12*60+D12)/1440</f>
         <v>12.88125</v>
       </c>
       <c r="F12" s="1">
@@ -2045,7 +2057,7 @@
         <v>3.9</v>
       </c>
       <c r="G17">
-        <f t="shared" ref="G17:G19" si="6">E17-5.366*4</f>
+        <f t="shared" ref="G17:G20" si="6">E17-5.366*4</f>
         <v>1.30961111111111</v>
       </c>
     </row>
@@ -2097,6 +2109,31 @@
       <c r="G19">
         <f t="shared" si="6"/>
         <v>5.32141666666667</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2">
+        <v>43057</v>
+      </c>
+      <c r="B20">
+        <v>29</v>
+      </c>
+      <c r="C20">
+        <v>21</v>
+      </c>
+      <c r="D20">
+        <v>55</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="4"/>
+        <v>29.9131944444444</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="G20">
+        <f>E20-5.366*5</f>
+        <v>3.08319444444444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Cep delta data.
</commit_message>
<xml_diff>
--- a/delta_cep/delta_cep.xlsx
+++ b/delta_cep/delta_cep.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="10935"/>
+    <workbookView windowWidth="16980" windowHeight="10935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,52 +16,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9">
   <si>
     <t>日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>相对日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>时</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>分</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>相对日数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>亮度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>日期相位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>周期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>年份</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.0_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,21 +65,352 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -92,9 +418,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -109,10 +677,57 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -159,6 +774,7 @@
               <a:rPr lang="en-US" altLang="zh-CN"/>
               <a:t>Cep delta</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -176,17 +792,26 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="marker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>2017</c:v>
+            <c:strRef>
+              <c:f>2017</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2017</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
               <a:noFill/>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -198,14 +823,19 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$G$2:$G$45</c:f>
@@ -213,31 +843,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
                 <c:pt idx="0">
-                  <c:v>0.76597222222222205</c:v>
+                  <c:v>0.765972222222222</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.82361111111111</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9083333333333301</c:v>
+                  <c:v>2.90833333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8576388888888902</c:v>
+                  <c:v>3.85763888888889</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>4.20046296296296</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.46663888888888899</c:v>
+                  <c:v>0.466638888888889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4763611111111099</c:v>
+                  <c:v>1.47636111111111</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5562222222222202</c:v>
+                  <c:v>2.55622222222222</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.4402499999999998</c:v>
+                  <c:v>4.44025</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.186055555555557</c:v>
@@ -246,34 +876,34 @@
                   <c:v>1.16591666666667</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.1492499999999999</c:v>
+                  <c:v>2.14925</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.1804999999999999</c:v>
+                  <c:v>3.1805</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.65686111111111201</c:v>
+                  <c:v>0.656861111111112</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>3.73463888888889</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.6797777777777796</c:v>
+                  <c:v>4.67977777777778</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.3096111111111099</c:v>
+                  <c:v>1.30961111111111</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>2.28322222222222</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.3214166666666696</c:v>
+                  <c:v>5.32141666666667</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.0831944444444401</c:v>
+                  <c:v>3.08319444444444</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.0109722222222297</c:v>
+                  <c:v>5.01097222222223</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>2.59497222222222</c:v>
@@ -282,10 +912,10 @@
                   <c:v>0.185916666666671</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.2755000000000001</c:v>
+                  <c:v>1.2755</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.2942500000000097</c:v>
+                  <c:v>5.29425000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>3.88866666666667</c:v>
@@ -294,10 +924,10 @@
                   <c:v>1.631</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.4434999999999998</c:v>
+                  <c:v>2.4435</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.6275277777777801</c:v>
+                  <c:v>2.62752777777778</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>3.45738888888889</c:v>
@@ -306,40 +936,40 @@
                   <c:v>4.53586111111112</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.2573611111111198</c:v>
+                  <c:v>4.25736111111112</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5.1809722222222199</c:v>
+                  <c:v>5.18097222222222</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.81775000000000397</c:v>
+                  <c:v>0.817750000000004</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>1.80802777777778</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.8031666666666699</c:v>
+                  <c:v>2.80316666666667</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.9323333333333399</c:v>
+                  <c:v>3.93233333333334</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.8642777777777804</c:v>
+                  <c:v>4.86427777777778</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>1.36147222222223</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.4857777777777801</c:v>
+                  <c:v>2.48577777777778</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.4906388888888999</c:v>
+                  <c:v>3.4906388888889</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>4.01769444444444</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.97177777777778795</c:v>
+                  <c:v>0.971777777777788</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>1.97108333333334</c:v>
@@ -372,7 +1002,7 @@
                   <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0999999999999996</c:v>
+                  <c:v>4.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>4.3</c:v>
@@ -483,7 +1113,7 @@
                   <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.0999999999999996</c:v>
+                  <c:v>4.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -494,11 +1124,20 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>2018</c:v>
+            <c:strRef>
+              <c:f>2018</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
               <a:noFill/>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -510,34 +1149,45 @@
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$46</c:f>
+              <c:f>Sheet1!$G$46:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4.6173611111111699</c:v>
+                  <c:v>4.61736111111117</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.23538888888891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$46</c:f>
+              <c:f>Sheet1!$F$46:$F$47</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -571,6 +1221,7 @@
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -589,6 +1240,7 @@
                 <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:prstDash val="solid"/>
             <a:round/>
           </a:ln>
           <a:effectLst/>
@@ -610,7 +1262,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="58113408"/>
@@ -635,6 +1286,7 @@
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -653,6 +1305,7 @@
                 <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:prstDash val="solid"/>
             <a:round/>
           </a:ln>
           <a:effectLst/>
@@ -674,7 +1327,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="58111104"/>
@@ -719,7 +1371,6 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -738,6 +1389,7 @@
           <a:lumOff val="85000"/>
         </a:schemeClr>
       </a:solidFill>
+      <a:prstDash val="solid"/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -749,643 +1401,6 @@
       <a:pPr>
         <a:defRPr lang="zh-CN"/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr defTabSz="914400">
-              <a:defRPr lang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>Cep delta</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>2017</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$G$2:$G$45</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="44"/>
-                <c:pt idx="0">
-                  <c:v>0.76597222222222205</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.82361111111111</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.9083333333333301</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.8576388888888902</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.20046296296296</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.46663888888888899</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.4763611111111099</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.5562222222222202</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.4402499999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.186055555555557</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.16591666666667</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.1492499999999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.1804999999999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.65686111111111201</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.73463888888889</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4.6797777777777796</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.3096111111111099</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.28322222222222</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5.3214166666666696</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.0831944444444401</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>5.0109722222222297</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.59497222222222</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.185916666666671</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.2755000000000001</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>5.2942500000000097</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3.88866666666667</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.631</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2.4434999999999998</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2.6275277777777801</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3.45738888888889</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>4.53586111111112</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>4.2573611111111198</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>5.1809722222222199</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.81775000000000397</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1.80802777777778</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2.8031666666666699</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3.9323333333333399</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>4.8642777777777804</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1.36147222222223</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2.4857777777777801</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3.4906388888888999</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>4.01769444444444</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.97177777777778795</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>1.97108333333334</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$F$2:$F$45</c:f>
-              <c:numCache>
-                <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="44"/>
-                <c:pt idx="0">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.9</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4.2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>4.3</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.9</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>4.3</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3.3</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>4.2</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>4.0999999999999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>2018</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$G$46</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>4.6173611111111699</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$F$46</c:f>
-              <c:numCache>
-                <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>3.4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="92394240"/>
-        <c:axId val="92396160"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="92394240"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="t"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="92396160"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.5"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="92396160"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-          <c:min val="3"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.0_ " sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="92394240"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.1"/>
-        <c:minorUnit val="0.05"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr lang="zh-CN"/>
-      </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1397,7 +1412,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
@@ -1407,55 +1422,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:colOff>666115</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>55880</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="图表 2"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>683260</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>168910</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>310515</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>81915</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="图表 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="5362575" y="142875"/>
+        <a:ext cx="6790690" cy="5742305"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1749,19 +1727,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9.125"/>
     <col min="2" max="2" width="8.75" customWidth="1"/>
@@ -1773,7 +1751,7 @@
     <col min="9" max="9" width="5.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1802,7 +1780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" s="2">
         <v>43028</v>
       </c>
@@ -1817,20 +1795,20 @@
       </c>
       <c r="E2">
         <f>(B2*1440+C2*60+D2)/1440</f>
-        <v>0.76597222222222205</v>
+        <v>0.765972222222222</v>
       </c>
       <c r="F2" s="1">
         <v>3.6</v>
       </c>
       <c r="G2">
         <f>E2</f>
-        <v>0.76597222222222205</v>
+        <v>0.765972222222222</v>
       </c>
       <c r="I2">
         <v>2017</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>43029</v>
       </c>
@@ -1855,7 +1833,7 @@
         <v>1.82361111111111</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>43030</v>
       </c>
@@ -1870,17 +1848,17 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>2.9083333333333301</v>
+        <v>2.90833333333333</v>
       </c>
       <c r="F4" s="1">
         <v>4.2</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>2.9083333333333301</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+        <v>2.90833333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2">
         <v>43031</v>
       </c>
@@ -1895,20 +1873,20 @@
       </c>
       <c r="E5">
         <f>(B5*1440+C5*60+D5)/1440</f>
-        <v>3.8576388888888888</v>
+        <v>3.85763888888889</v>
       </c>
       <c r="F5" s="1">
         <v>3.4</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>3.8576388888888902</v>
+        <v>3.85763888888889</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>43032</v>
       </c>
@@ -1933,7 +1911,7 @@
         <v>4.20046296296296</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>43033</v>
       </c>
@@ -1948,17 +1926,17 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>5.8326388888888898</v>
+        <v>5.83263888888889</v>
       </c>
       <c r="F7" s="1">
         <v>3.7</v>
       </c>
       <c r="G7">
         <f>E7-5.366</f>
-        <v>0.46663888888888899</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+        <v>0.466638888888889</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>43034</v>
       </c>
@@ -1976,14 +1954,14 @@
         <v>6.84236111111111</v>
       </c>
       <c r="F8" s="1">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="G8">
         <f t="shared" ref="G8:G10" si="2">E8-5.366</f>
-        <v>1.4763611111111099</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+        <v>1.47636111111111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>43035</v>
       </c>
@@ -1998,17 +1976,17 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>7.9222222222222198</v>
+        <v>7.92222222222222</v>
       </c>
       <c r="F9" s="1">
         <v>4.3</v>
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>2.5562222222222202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+        <v>2.55622222222222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="2">
         <v>43037</v>
       </c>
@@ -2023,20 +2001,20 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>9.8062500000000004</v>
+        <v>9.80625</v>
       </c>
       <c r="F10" s="1">
         <v>3.4</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>4.4402499999999998</v>
+        <v>4.44025</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>43038</v>
       </c>
@@ -2061,7 +2039,7 @@
         <v>0.186055555555557</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>43039</v>
       </c>
@@ -2076,7 +2054,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>11.897916666666699</v>
+        <v>11.8979166666667</v>
       </c>
       <c r="F12" s="1">
         <v>3.8</v>
@@ -2086,7 +2064,7 @@
         <v>1.16591666666667</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>43040</v>
       </c>
@@ -2100,7 +2078,7 @@
         <v>9</v>
       </c>
       <c r="E13">
-        <f t="shared" ref="E13:E44" si="4">(B13*1440+C13*60+D13)/1440</f>
+        <f t="shared" ref="E13:E47" si="4">(B13*1440+C13*60+D13)/1440</f>
         <v>12.88125</v>
       </c>
       <c r="F13" s="1">
@@ -2108,10 +2086,10 @@
       </c>
       <c r="G13">
         <f t="shared" si="3"/>
-        <v>2.1492499999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+        <v>2.14925</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2">
         <v>43041</v>
       </c>
@@ -2133,10 +2111,10 @@
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
-        <v>3.1804999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+        <v>3.1805</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="2">
         <v>43044</v>
       </c>
@@ -2151,20 +2129,20 @@
       </c>
       <c r="E15">
         <f t="shared" si="4"/>
-        <v>16.754861111111101</v>
+        <v>16.7548611111111</v>
       </c>
       <c r="F15" s="1">
         <v>3.5</v>
       </c>
       <c r="G15">
         <f t="shared" ref="G15:G17" si="5">E15-5.366*3</f>
-        <v>0.65686111111111201</v>
+        <v>0.656861111111112</v>
       </c>
       <c r="H15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7">
       <c r="A16" s="2">
         <v>43047</v>
       </c>
@@ -2179,7 +2157,7 @@
       </c>
       <c r="E16">
         <f t="shared" si="4"/>
-        <v>19.832638888888901</v>
+        <v>19.8326388888889</v>
       </c>
       <c r="F16" s="1">
         <v>3.7</v>
@@ -2189,7 +2167,7 @@
         <v>3.73463888888889</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7">
       <c r="A17" s="2">
         <v>43048</v>
       </c>
@@ -2211,10 +2189,10 @@
       </c>
       <c r="G17">
         <f t="shared" si="5"/>
-        <v>4.6797777777777796</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+        <v>4.67977777777778</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="2">
         <v>43050</v>
       </c>
@@ -2229,17 +2207,17 @@
       </c>
       <c r="E18">
         <f t="shared" si="4"/>
-        <v>22.773611111111101</v>
+        <v>22.7736111111111</v>
       </c>
       <c r="F18" s="1">
         <v>3.9</v>
       </c>
       <c r="G18">
         <f t="shared" ref="G18:G20" si="6">E18-5.366*4</f>
-        <v>1.3096111111111099</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+        <v>1.30961111111111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="2">
         <v>43051</v>
       </c>
@@ -2254,7 +2232,7 @@
       </c>
       <c r="E19">
         <f t="shared" si="4"/>
-        <v>23.747222222222199</v>
+        <v>23.7472222222222</v>
       </c>
       <c r="F19" s="1">
         <v>4.2</v>
@@ -2264,7 +2242,7 @@
         <v>2.28322222222222</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8">
       <c r="A20" s="2">
         <v>43054</v>
       </c>
@@ -2279,20 +2257,20 @@
       </c>
       <c r="E20">
         <f t="shared" si="4"/>
-        <v>26.785416666666698</v>
+        <v>26.7854166666667</v>
       </c>
       <c r="F20" s="1">
         <v>3.5</v>
       </c>
       <c r="G20">
         <f t="shared" si="6"/>
-        <v>5.3214166666666696</v>
+        <v>5.32141666666667</v>
       </c>
       <c r="H20">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
         <v>43057</v>
       </c>
@@ -2314,10 +2292,10 @@
       </c>
       <c r="G21">
         <f t="shared" ref="G21:G22" si="7">E21-5.366*5</f>
-        <v>3.0831944444444401</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+        <v>3.08319444444444</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="2">
         <v>43059</v>
       </c>
@@ -2332,20 +2310,20 @@
       </c>
       <c r="E22">
         <f t="shared" si="4"/>
-        <v>31.840972222222199</v>
+        <v>31.8409722222222</v>
       </c>
       <c r="F22" s="1">
         <v>3.4</v>
       </c>
       <c r="G22">
         <f t="shared" si="7"/>
-        <v>5.0109722222222297</v>
+        <v>5.01097222222223</v>
       </c>
       <c r="H22">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7">
       <c r="A23" s="2">
         <v>43062</v>
       </c>
@@ -2360,7 +2338,7 @@
       </c>
       <c r="E23">
         <f t="shared" si="4"/>
-        <v>34.790972222222202</v>
+        <v>34.7909722222222</v>
       </c>
       <c r="F23" s="1">
         <v>4</v>
@@ -2370,7 +2348,7 @@
         <v>2.59497222222222</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8">
       <c r="A24" s="2">
         <v>43065</v>
       </c>
@@ -2385,7 +2363,7 @@
       </c>
       <c r="E24">
         <f t="shared" si="4"/>
-        <v>37.747916666666697</v>
+        <v>37.7479166666667</v>
       </c>
       <c r="F24" s="1">
         <v>3.5</v>
@@ -2398,7 +2376,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7">
       <c r="A25" s="2">
         <v>43066</v>
       </c>
@@ -2413,17 +2391,17 @@
       </c>
       <c r="E25">
         <f t="shared" si="4"/>
-        <v>38.837499999999999</v>
+        <v>38.8375</v>
       </c>
       <c r="F25" s="1">
         <v>3.7</v>
       </c>
       <c r="G25">
         <f t="shared" si="8"/>
-        <v>1.2755000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+        <v>1.2755</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="2">
         <v>43070</v>
       </c>
@@ -2438,20 +2416,20 @@
       </c>
       <c r="E26">
         <f t="shared" si="4"/>
-        <v>42.856250000000003</v>
+        <v>42.85625</v>
       </c>
       <c r="F26" s="1">
         <v>3.4</v>
       </c>
       <c r="G26">
         <f t="shared" si="8"/>
-        <v>5.2942500000000097</v>
+        <v>5.29425000000001</v>
       </c>
       <c r="H26">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8">
       <c r="A27" s="2">
         <v>43074</v>
       </c>
@@ -2466,7 +2444,7 @@
       </c>
       <c r="E27">
         <f t="shared" si="4"/>
-        <v>46.816666666666698</v>
+        <v>46.8166666666667</v>
       </c>
       <c r="F27" s="1">
         <v>3.4</v>
@@ -2479,7 +2457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7">
       <c r="A28" s="2">
         <v>43077</v>
       </c>
@@ -2495,7 +2473,7 @@
       </c>
       <c r="E28">
         <f t="shared" si="4"/>
-        <v>49.924999999999997</v>
+        <v>49.925</v>
       </c>
       <c r="F28" s="1">
         <v>4</v>
@@ -2505,7 +2483,7 @@
         <v>1.631</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7">
       <c r="A29" s="2">
         <v>43078</v>
       </c>
@@ -2520,17 +2498,17 @@
       </c>
       <c r="E29">
         <f t="shared" si="4"/>
-        <v>50.737499999999997</v>
+        <v>50.7375</v>
       </c>
       <c r="F29" s="1">
         <v>4.2</v>
       </c>
       <c r="G29">
         <f t="shared" si="9"/>
-        <v>2.4434999999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+        <v>2.4435</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="2">
         <v>43078</v>
       </c>
@@ -2545,17 +2523,17 @@
       </c>
       <c r="E30">
         <f t="shared" si="4"/>
-        <v>50.921527777777797</v>
+        <v>50.9215277777778</v>
       </c>
       <c r="F30" s="1">
         <v>4.3</v>
       </c>
       <c r="G30">
         <f t="shared" si="9"/>
-        <v>2.6275277777777801</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+        <v>2.62752777777778</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="2">
         <v>43079</v>
       </c>
@@ -2570,7 +2548,7 @@
       </c>
       <c r="E31">
         <f t="shared" si="4"/>
-        <v>51.751388888888897</v>
+        <v>51.7513888888889</v>
       </c>
       <c r="F31" s="1">
         <v>4</v>
@@ -2580,7 +2558,7 @@
         <v>3.45738888888889</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8">
       <c r="A32" s="2">
         <v>43080</v>
       </c>
@@ -2608,7 +2586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8">
       <c r="A33" s="2">
         <v>43085</v>
       </c>
@@ -2623,20 +2601,20 @@
       </c>
       <c r="E33">
         <f t="shared" si="4"/>
-        <v>57.917361111111099</v>
+        <v>57.9173611111111</v>
       </c>
       <c r="F33" s="1">
         <v>3.5</v>
       </c>
       <c r="G33">
         <f t="shared" ref="G33:G34" si="10">E33-5.366*10</f>
-        <v>4.2573611111111198</v>
+        <v>4.25736111111112</v>
       </c>
       <c r="H33">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7">
       <c r="A34" s="2">
         <v>43086</v>
       </c>
@@ -2651,17 +2629,17 @@
       </c>
       <c r="E34">
         <f t="shared" si="4"/>
-        <v>58.840972222222199</v>
+        <v>58.8409722222222</v>
       </c>
       <c r="F34" s="1">
         <v>3.7</v>
       </c>
       <c r="G34">
         <f t="shared" si="10"/>
-        <v>5.1809722222222199</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+        <v>5.18097222222222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="2">
         <v>43087</v>
       </c>
@@ -2683,10 +2661,10 @@
       </c>
       <c r="G35">
         <f t="shared" ref="G35:G39" si="11">E35-5.366*11</f>
-        <v>0.81775000000000397</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+        <v>0.817750000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="2">
         <v>43088</v>
       </c>
@@ -2701,7 +2679,7 @@
       </c>
       <c r="E36">
         <f t="shared" si="4"/>
-        <v>60.834027777777798</v>
+        <v>60.8340277777778</v>
       </c>
       <c r="F36" s="1">
         <v>4</v>
@@ -2711,7 +2689,7 @@
         <v>1.80802777777778</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7">
       <c r="A37" s="2">
         <v>43089</v>
       </c>
@@ -2726,17 +2704,17 @@
       </c>
       <c r="E37">
         <f t="shared" si="4"/>
-        <v>61.829166666666701</v>
+        <v>61.8291666666667</v>
       </c>
       <c r="F37" s="1">
         <v>4.3</v>
       </c>
       <c r="G37">
         <f t="shared" si="11"/>
-        <v>2.8031666666666699</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+        <v>2.80316666666667</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="2">
         <v>43090</v>
       </c>
@@ -2758,13 +2736,13 @@
       </c>
       <c r="G38">
         <f t="shared" si="11"/>
-        <v>3.9323333333333399</v>
+        <v>3.93233333333334</v>
       </c>
       <c r="H38">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7">
       <c r="A39" s="2">
         <v>43091</v>
       </c>
@@ -2779,17 +2757,17 @@
       </c>
       <c r="E39">
         <f t="shared" si="4"/>
-        <v>63.890277777777797</v>
+        <v>63.8902777777778</v>
       </c>
       <c r="F39" s="1">
         <v>3.5</v>
       </c>
       <c r="G39">
         <f t="shared" si="11"/>
-        <v>4.8642777777777804</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+        <v>4.86427777777778</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="2">
         <v>43093</v>
       </c>
@@ -2815,7 +2793,7 @@
         <v>1.36147222222223</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:7">
       <c r="A41" s="2">
         <v>43094</v>
       </c>
@@ -2830,17 +2808,17 @@
       </c>
       <c r="E41">
         <f t="shared" si="4"/>
-        <v>66.877777777777794</v>
+        <v>66.8777777777778</v>
       </c>
       <c r="F41" s="1">
         <v>4.2</v>
       </c>
       <c r="G41">
         <f t="shared" si="12"/>
-        <v>2.4857777777777801</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+        <v>2.48577777777778</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="2">
         <v>43095</v>
       </c>
@@ -2855,17 +2833,17 @@
       </c>
       <c r="E42">
         <f t="shared" si="4"/>
-        <v>67.882638888888906</v>
+        <v>67.8826388888889</v>
       </c>
       <c r="F42" s="1">
         <v>4</v>
       </c>
       <c r="G42">
         <f t="shared" si="12"/>
-        <v>3.4906388888888999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+        <v>3.4906388888889</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="2">
         <v>43101</v>
       </c>
@@ -2881,7 +2859,7 @@
       </c>
       <c r="E43">
         <f t="shared" si="4"/>
-        <v>73.775694444444397</v>
+        <v>73.7756944444444</v>
       </c>
       <c r="F43" s="1">
         <v>3.5</v>
@@ -2897,7 +2875,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8">
       <c r="A44" s="2">
         <v>43114</v>
       </c>
@@ -2912,20 +2890,20 @@
       </c>
       <c r="E44">
         <f t="shared" si="4"/>
-        <v>86.827777777777797</v>
+        <v>86.8277777777778</v>
       </c>
       <c r="F44" s="1">
         <v>3.8</v>
       </c>
       <c r="G44">
         <f t="shared" ref="G44:G45" si="13">E44-5.366*16</f>
-        <v>0.97177777777778795</v>
+        <v>0.971777777777788</v>
       </c>
       <c r="H44">
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:7">
       <c r="A45" s="2">
         <v>43115</v>
       </c>
@@ -2939,18 +2917,18 @@
         <v>51</v>
       </c>
       <c r="E45">
-        <f>(B45*1440+C45*60+D45)/1440</f>
-        <v>87.827083333333306</v>
+        <f t="shared" si="4"/>
+        <v>87.8270833333333</v>
       </c>
       <c r="F45" s="1">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="G45">
         <f t="shared" si="13"/>
         <v>1.97108333333334</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8">
       <c r="A46" s="2">
         <v>43300</v>
       </c>
@@ -2965,53 +2943,85 @@
         <v>1</v>
       </c>
       <c r="E46">
-        <f>(B46*1440+C46*60+D46)/1440</f>
-        <v>272.91736111111101</v>
+        <f t="shared" si="4"/>
+        <v>272.917361111111</v>
       </c>
       <c r="F46" s="1">
         <v>3.4</v>
       </c>
       <c r="G46">
         <f>E46-5.366*50</f>
-        <v>4.6173611111111699</v>
+        <v>4.61736111111117</v>
       </c>
       <c r="H46">
         <v>50</v>
       </c>
     </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="2">
+        <v>43305</v>
+      </c>
+      <c r="B47">
+        <f>A47-A46+B46</f>
+        <v>277</v>
+      </c>
+      <c r="C47">
+        <v>21</v>
+      </c>
+      <c r="D47">
+        <v>38</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="4"/>
+        <v>277.901388888889</v>
+      </c>
+      <c r="F47" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="G47">
+        <f>E47-5.366*51</f>
+        <v>4.23538888888891</v>
+      </c>
+      <c r="H47">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add delta Cep + mu Cep data
</commit_message>
<xml_diff>
--- a/delta_cep/delta_cep.xlsx
+++ b/delta_cep/delta_cep.xlsx
@@ -7,8 +7,8 @@
     <workbookView windowWidth="16980" windowHeight="10935"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="delta_cep" sheetId="1" r:id="rId1"/>
+    <sheet name="mu_cep" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -62,11 +62,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.0_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -81,6 +81,14 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -122,8 +130,60 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -161,68 +221,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,7 +243,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -255,49 +261,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,6 +303,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -333,67 +357,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,13 +411,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,6 +428,54 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -442,15 +490,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -489,45 +528,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -536,10 +536,10 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -548,144 +548,150 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -860,7 +866,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$45</c:f>
+              <c:f>delta_cep!$G$2:$G$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
@@ -1001,7 +1007,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$45</c:f>
+              <c:f>delta_cep!$F$2:$F$45</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
                 <c:ptCount val="44"/>
@@ -1186,10 +1192,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$46:$G$61</c:f>
+              <c:f>delta_cep!$G$46:$G$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>4.61736111111117</c:v>
                 </c:pt>
@@ -1237,16 +1243,31 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>3.32622222222221</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.35538888888891</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.99286111111115</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.620611111111032</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.63033333333306</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.66019444444447</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$46:$F$61</c:f>
+              <c:f>delta_cep!$F$46:$F$66</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>3.4</c:v>
                 </c:pt>
@@ -1293,6 +1314,21 @@
                   <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -1839,10 +1875,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T42" sqref="T42"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1852,7 +1888,7 @@
     <col min="3" max="3" width="4.625" customWidth="1"/>
     <col min="4" max="4" width="4.875" customWidth="1"/>
     <col min="5" max="5" width="10.25" customWidth="1"/>
-    <col min="6" max="6" width="5.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.25" style="4" customWidth="1"/>
     <col min="7" max="7" width="12.625"/>
     <col min="8" max="9" width="4.625" customWidth="1"/>
   </cols>
@@ -1873,7 +1909,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -1887,7 +1923,7 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>43028</v>
       </c>
       <c r="B2">
@@ -1903,7 +1939,7 @@
         <f>(B2*1440+C2*60+D2)/1440</f>
         <v>0.765972222222222</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="4">
         <v>3.6</v>
       </c>
       <c r="G2">
@@ -1915,7 +1951,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>43029</v>
       </c>
       <c r="B3">
@@ -1931,7 +1967,7 @@
         <f t="shared" ref="E3:G12" si="0">(B3*1440+C3*60+D3)/1440</f>
         <v>1.82361111111111</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="4">
         <v>4</v>
       </c>
       <c r="G3">
@@ -1940,7 +1976,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>43030</v>
       </c>
       <c r="B4">
@@ -1956,7 +1992,7 @@
         <f t="shared" si="0"/>
         <v>2.90833333333333</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="4">
         <v>4.2</v>
       </c>
       <c r="G4">
@@ -1965,7 +2001,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>43031</v>
       </c>
       <c r="B5">
@@ -1981,7 +2017,7 @@
         <f>(B5*1440+C5*60+D5)/1440</f>
         <v>3.85763888888889</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="4">
         <v>3.4</v>
       </c>
       <c r="G5">
@@ -1993,7 +2029,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>43032</v>
       </c>
       <c r="B6">
@@ -2009,7 +2045,7 @@
         <f t="shared" si="0"/>
         <v>4.75277777777778</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="4">
         <v>3.5</v>
       </c>
       <c r="G6">
@@ -2018,7 +2054,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <v>43033</v>
       </c>
       <c r="B7">
@@ -2034,7 +2070,7 @@
         <f t="shared" si="0"/>
         <v>5.83263888888889</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="4">
         <v>3.7</v>
       </c>
       <c r="G7">
@@ -2043,7 +2079,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <v>43034</v>
       </c>
       <c r="B8">
@@ -2059,7 +2095,7 @@
         <f t="shared" si="0"/>
         <v>6.84236111111111</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="4">
         <v>4.1</v>
       </c>
       <c r="G8">
@@ -2068,7 +2104,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <v>43035</v>
       </c>
       <c r="B9">
@@ -2084,7 +2120,7 @@
         <f t="shared" si="0"/>
         <v>7.92222222222222</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="4">
         <v>4.3</v>
       </c>
       <c r="G9">
@@ -2093,7 +2129,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>43037</v>
       </c>
       <c r="B10">
@@ -2109,7 +2145,7 @@
         <f t="shared" si="0"/>
         <v>9.80625</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="4">
         <v>3.4</v>
       </c>
       <c r="G10">
@@ -2121,7 +2157,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>43038</v>
       </c>
       <c r="B11">
@@ -2137,7 +2173,7 @@
         <f t="shared" si="0"/>
         <v>10.9180555555556</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="4">
         <v>3.6</v>
       </c>
       <c r="G11">
@@ -2146,7 +2182,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="2">
+      <c r="A12" s="3">
         <v>43039</v>
       </c>
       <c r="B12">
@@ -2162,7 +2198,7 @@
         <f t="shared" si="0"/>
         <v>11.8979166666667</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="4">
         <v>3.8</v>
       </c>
       <c r="G12">
@@ -2171,7 +2207,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="2">
+      <c r="A13" s="3">
         <v>43040</v>
       </c>
       <c r="B13">
@@ -2184,10 +2220,10 @@
         <v>9</v>
       </c>
       <c r="E13">
-        <f t="shared" ref="E13:E61" si="4">(B13*1440+C13*60+D13)/1440</f>
+        <f t="shared" ref="E13:E66" si="4">(B13*1440+C13*60+D13)/1440</f>
         <v>12.88125</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="4">
         <v>4</v>
       </c>
       <c r="G13">
@@ -2196,7 +2232,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="2">
+      <c r="A14" s="3">
         <v>43041</v>
       </c>
       <c r="B14">
@@ -2212,7 +2248,7 @@
         <f t="shared" si="4"/>
         <v>13.9125</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="4">
         <v>3.7</v>
       </c>
       <c r="G14">
@@ -2221,7 +2257,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="2">
+      <c r="A15" s="3">
         <v>43044</v>
       </c>
       <c r="B15">
@@ -2237,7 +2273,7 @@
         <f t="shared" si="4"/>
         <v>16.7548611111111</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="4">
         <v>3.5</v>
       </c>
       <c r="G15">
@@ -2249,7 +2285,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="2">
+      <c r="A16" s="3">
         <v>43047</v>
       </c>
       <c r="B16">
@@ -2265,7 +2301,7 @@
         <f t="shared" si="4"/>
         <v>19.8326388888889</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="4">
         <v>3.7</v>
       </c>
       <c r="G16">
@@ -2274,7 +2310,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="2">
+      <c r="A17" s="3">
         <v>43048</v>
       </c>
       <c r="B17">
@@ -2290,7 +2326,7 @@
         <f t="shared" si="4"/>
         <v>20.7777777777778</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="4">
         <v>3.5</v>
       </c>
       <c r="G17">
@@ -2299,7 +2335,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="2">
+      <c r="A18" s="3">
         <v>43050</v>
       </c>
       <c r="B18">
@@ -2315,7 +2351,7 @@
         <f t="shared" si="4"/>
         <v>22.7736111111111</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="4">
         <v>3.9</v>
       </c>
       <c r="G18">
@@ -2324,7 +2360,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="2">
+      <c r="A19" s="3">
         <v>43051</v>
       </c>
       <c r="B19">
@@ -2340,7 +2376,7 @@
         <f t="shared" si="4"/>
         <v>23.7472222222222</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="4">
         <v>4.2</v>
       </c>
       <c r="G19">
@@ -2349,7 +2385,7 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="2">
+      <c r="A20" s="3">
         <v>43054</v>
       </c>
       <c r="B20">
@@ -2365,7 +2401,7 @@
         <f t="shared" si="4"/>
         <v>26.7854166666667</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="4">
         <v>3.5</v>
       </c>
       <c r="G20">
@@ -2377,7 +2413,7 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="2">
+      <c r="A21" s="3">
         <v>43057</v>
       </c>
       <c r="B21">
@@ -2393,7 +2429,7 @@
         <f t="shared" si="4"/>
         <v>29.9131944444444</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="4">
         <v>3.8</v>
       </c>
       <c r="G21">
@@ -2402,7 +2438,7 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="2">
+      <c r="A22" s="3">
         <v>43059</v>
       </c>
       <c r="B22">
@@ -2418,7 +2454,7 @@
         <f t="shared" si="4"/>
         <v>31.8409722222222</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="4">
         <v>3.4</v>
       </c>
       <c r="G22">
@@ -2430,7 +2466,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="2">
+      <c r="A23" s="3">
         <v>43062</v>
       </c>
       <c r="B23">
@@ -2446,7 +2482,7 @@
         <f t="shared" si="4"/>
         <v>34.7909722222222</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="4">
         <v>4</v>
       </c>
       <c r="G23">
@@ -2455,7 +2491,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="2">
+      <c r="A24" s="3">
         <v>43065</v>
       </c>
       <c r="B24">
@@ -2471,7 +2507,7 @@
         <f t="shared" si="4"/>
         <v>37.7479166666667</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="4">
         <v>3.5</v>
       </c>
       <c r="G24">
@@ -2483,7 +2519,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="2">
+      <c r="A25" s="3">
         <v>43066</v>
       </c>
       <c r="B25">
@@ -2499,7 +2535,7 @@
         <f t="shared" si="4"/>
         <v>38.8375</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="4">
         <v>3.7</v>
       </c>
       <c r="G25">
@@ -2508,7 +2544,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="2">
+      <c r="A26" s="3">
         <v>43070</v>
       </c>
       <c r="B26">
@@ -2524,7 +2560,7 @@
         <f t="shared" si="4"/>
         <v>42.85625</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="4">
         <v>3.4</v>
       </c>
       <c r="G26">
@@ -2536,7 +2572,7 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="2">
+      <c r="A27" s="3">
         <v>43074</v>
       </c>
       <c r="B27">
@@ -2552,7 +2588,7 @@
         <f t="shared" si="4"/>
         <v>46.8166666666667</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="4">
         <v>3.4</v>
       </c>
       <c r="G27">
@@ -2564,7 +2600,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="2">
+      <c r="A28" s="3">
         <v>43077</v>
       </c>
       <c r="B28">
@@ -2581,7 +2617,7 @@
         <f t="shared" si="4"/>
         <v>49.925</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="4">
         <v>4</v>
       </c>
       <c r="G28">
@@ -2590,7 +2626,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="2">
+      <c r="A29" s="3">
         <v>43078</v>
       </c>
       <c r="B29">
@@ -2606,7 +2642,7 @@
         <f t="shared" si="4"/>
         <v>50.7375</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="4">
         <v>4.2</v>
       </c>
       <c r="G29">
@@ -2615,7 +2651,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="2">
+      <c r="A30" s="3">
         <v>43078</v>
       </c>
       <c r="B30">
@@ -2631,7 +2667,7 @@
         <f t="shared" si="4"/>
         <v>50.9215277777778</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="4">
         <v>4.3</v>
       </c>
       <c r="G30">
@@ -2640,7 +2676,7 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="2">
+      <c r="A31" s="3">
         <v>43079</v>
       </c>
       <c r="B31">
@@ -2656,7 +2692,7 @@
         <f t="shared" si="4"/>
         <v>51.7513888888889</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="4">
         <v>4</v>
       </c>
       <c r="G31">
@@ -2665,7 +2701,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="2">
+      <c r="A32" s="3">
         <v>43080</v>
       </c>
       <c r="B32">
@@ -2681,7 +2717,7 @@
         <f t="shared" si="4"/>
         <v>52.8298611111111</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="4">
         <v>3.4</v>
       </c>
       <c r="G32">
@@ -2693,7 +2729,7 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="2">
+      <c r="A33" s="3">
         <v>43085</v>
       </c>
       <c r="B33">
@@ -2709,7 +2745,7 @@
         <f t="shared" si="4"/>
         <v>57.9173611111111</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="4">
         <v>3.5</v>
       </c>
       <c r="G33">
@@ -2721,7 +2757,7 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="2">
+      <c r="A34" s="3">
         <v>43086</v>
       </c>
       <c r="B34">
@@ -2737,7 +2773,7 @@
         <f t="shared" si="4"/>
         <v>58.8409722222222</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="4">
         <v>3.7</v>
       </c>
       <c r="G34">
@@ -2746,7 +2782,7 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="2">
+      <c r="A35" s="3">
         <v>43087</v>
       </c>
       <c r="B35">
@@ -2762,7 +2798,7 @@
         <f t="shared" si="4"/>
         <v>59.84375</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35" s="4">
         <v>3.9</v>
       </c>
       <c r="G35">
@@ -2771,7 +2807,7 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="2">
+      <c r="A36" s="3">
         <v>43088</v>
       </c>
       <c r="B36">
@@ -2787,7 +2823,7 @@
         <f t="shared" si="4"/>
         <v>60.8340277777778</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36" s="4">
         <v>4</v>
       </c>
       <c r="G36">
@@ -2796,7 +2832,7 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="2">
+      <c r="A37" s="3">
         <v>43089</v>
       </c>
       <c r="B37">
@@ -2812,7 +2848,7 @@
         <f t="shared" si="4"/>
         <v>61.8291666666667</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F37" s="4">
         <v>4.3</v>
       </c>
       <c r="G37">
@@ -2821,7 +2857,7 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="2">
+      <c r="A38" s="3">
         <v>43090</v>
       </c>
       <c r="B38">
@@ -2837,7 +2873,7 @@
         <f t="shared" si="4"/>
         <v>62.9583333333333</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38" s="4">
         <v>3.3</v>
       </c>
       <c r="G38">
@@ -2849,7 +2885,7 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="2">
+      <c r="A39" s="3">
         <v>43091</v>
       </c>
       <c r="B39">
@@ -2865,7 +2901,7 @@
         <f t="shared" si="4"/>
         <v>63.8902777777778</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39" s="4">
         <v>3.5</v>
       </c>
       <c r="G39">
@@ -2874,7 +2910,7 @@
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="2">
+      <c r="A40" s="3">
         <v>43093</v>
       </c>
       <c r="B40">
@@ -2891,7 +2927,7 @@
         <f t="shared" si="4"/>
         <v>65.7534722222222</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40" s="4">
         <v>4</v>
       </c>
       <c r="G40">
@@ -2900,7 +2936,7 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="2">
+      <c r="A41" s="3">
         <v>43094</v>
       </c>
       <c r="B41">
@@ -2916,7 +2952,7 @@
         <f t="shared" si="4"/>
         <v>66.8777777777778</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41" s="4">
         <v>4.2</v>
       </c>
       <c r="G41">
@@ -2925,7 +2961,7 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="2">
+      <c r="A42" s="3">
         <v>43095</v>
       </c>
       <c r="B42">
@@ -2941,7 +2977,7 @@
         <f t="shared" si="4"/>
         <v>67.8826388888889</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42" s="4">
         <v>4</v>
       </c>
       <c r="G42">
@@ -2950,7 +2986,7 @@
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="2">
+      <c r="A43" s="3">
         <v>43101</v>
       </c>
       <c r="B43">
@@ -2967,7 +3003,7 @@
         <f t="shared" si="4"/>
         <v>73.7756944444444</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F43" s="4">
         <v>3.5</v>
       </c>
       <c r="G43">
@@ -2982,7 +3018,7 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="2">
+      <c r="A44" s="3">
         <v>43114</v>
       </c>
       <c r="B44">
@@ -2998,7 +3034,7 @@
         <f t="shared" si="4"/>
         <v>86.8277777777778</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F44" s="4">
         <v>3.8</v>
       </c>
       <c r="G44">
@@ -3010,7 +3046,7 @@
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="2">
+      <c r="A45" s="3">
         <v>43115</v>
       </c>
       <c r="B45">
@@ -3026,7 +3062,7 @@
         <f t="shared" si="4"/>
         <v>87.8270833333333</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F45" s="4">
         <v>4.1</v>
       </c>
       <c r="G45">
@@ -3035,11 +3071,11 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="2">
+      <c r="A46" s="3">
         <v>43300</v>
       </c>
       <c r="B46">
-        <f t="shared" ref="B46:B61" si="14">A46-A45+B45</f>
+        <f t="shared" ref="B46:B66" si="14">A46-A45+B45</f>
         <v>272</v>
       </c>
       <c r="C46">
@@ -3052,7 +3088,7 @@
         <f t="shared" si="4"/>
         <v>272.917361111111</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F46" s="4">
         <v>3.4</v>
       </c>
       <c r="G46">
@@ -3064,7 +3100,7 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="2">
+      <c r="A47" s="3">
         <v>43305</v>
       </c>
       <c r="B47">
@@ -3081,7 +3117,7 @@
         <f t="shared" si="4"/>
         <v>277.901388888889</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F47" s="4">
         <v>3.3</v>
       </c>
       <c r="G47">
@@ -3093,7 +3129,7 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="2">
+      <c r="A48" s="3">
         <v>43311</v>
       </c>
       <c r="B48">
@@ -3110,7 +3146,7 @@
         <f t="shared" si="4"/>
         <v>283.893055555556</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F48" s="4">
         <v>3.4</v>
       </c>
       <c r="G48">
@@ -3122,7 +3158,7 @@
       </c>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="2">
+      <c r="A49" s="3">
         <v>43312</v>
       </c>
       <c r="B49">
@@ -3139,7 +3175,7 @@
         <f t="shared" si="4"/>
         <v>284.890972222222</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F49" s="4">
         <v>3.8</v>
       </c>
       <c r="G49">
@@ -3154,7 +3190,7 @@
       </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="2">
+      <c r="A50" s="3">
         <v>43313</v>
       </c>
       <c r="B50">
@@ -3171,7 +3207,7 @@
         <f t="shared" si="4"/>
         <v>285.861805555556</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F50" s="4">
         <v>3.9</v>
       </c>
       <c r="G50">
@@ -3183,7 +3219,7 @@
       </c>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="2">
+      <c r="A51" s="3">
         <v>43315</v>
       </c>
       <c r="B51">
@@ -3200,7 +3236,7 @@
         <f t="shared" si="4"/>
         <v>287.878472222222</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F51" s="4">
         <v>3.7</v>
       </c>
       <c r="G51">
@@ -3212,7 +3248,7 @@
       </c>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="2">
+      <c r="A52" s="3">
         <v>43316</v>
       </c>
       <c r="B52">
@@ -3229,7 +3265,7 @@
         <f t="shared" si="4"/>
         <v>288.859027777778</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F52" s="4">
         <v>3.4</v>
       </c>
       <c r="G52">
@@ -3241,7 +3277,7 @@
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="2">
+      <c r="A53" s="3">
         <v>43317</v>
       </c>
       <c r="B53">
@@ -3258,7 +3294,7 @@
         <f t="shared" si="4"/>
         <v>289.845833333333</v>
       </c>
-      <c r="F53" s="1">
+      <c r="F53" s="4">
         <v>3.5</v>
       </c>
       <c r="G53">
@@ -3273,7 +3309,7 @@
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="2">
+      <c r="A54" s="3">
         <v>43319</v>
       </c>
       <c r="B54">
@@ -3290,7 +3326,7 @@
         <f t="shared" si="4"/>
         <v>291.052777777778</v>
       </c>
-      <c r="F54" s="1">
+      <c r="F54" s="4">
         <v>3.9</v>
       </c>
       <c r="G54">
@@ -3299,7 +3335,7 @@
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="2">
+      <c r="A55" s="3">
         <v>43319</v>
       </c>
       <c r="B55">
@@ -3316,7 +3352,7 @@
         <f t="shared" si="4"/>
         <v>291.870833333333</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F55" s="4">
         <v>4.1</v>
       </c>
       <c r="G55">
@@ -3328,7 +3364,7 @@
       </c>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="2">
+      <c r="A56" s="3">
         <v>43320</v>
       </c>
       <c r="B56">
@@ -3345,7 +3381,7 @@
         <f t="shared" si="4"/>
         <v>292.850694444444</v>
       </c>
-      <c r="F56" s="1">
+      <c r="F56" s="4">
         <v>4.2</v>
       </c>
       <c r="G56">
@@ -3357,7 +3393,7 @@
       </c>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="2">
+      <c r="A57" s="3">
         <v>43321</v>
       </c>
       <c r="B57">
@@ -3374,7 +3410,7 @@
         <f t="shared" si="4"/>
         <v>293.852777777778</v>
       </c>
-      <c r="F57" s="1">
+      <c r="F57" s="4">
         <v>3.4</v>
       </c>
       <c r="G57">
@@ -3386,7 +3422,7 @@
       </c>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="2">
+      <c r="A58" s="3">
         <v>43322</v>
       </c>
       <c r="B58">
@@ -3403,7 +3439,7 @@
         <f t="shared" si="4"/>
         <v>294.860416666667</v>
       </c>
-      <c r="F58" s="1">
+      <c r="F58" s="4">
         <v>3.5</v>
       </c>
       <c r="G58">
@@ -3415,7 +3451,7 @@
       </c>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="2">
+      <c r="A59" s="3">
         <v>43325</v>
       </c>
       <c r="B59">
@@ -3432,7 +3468,7 @@
         <f t="shared" si="4"/>
         <v>297.85</v>
       </c>
-      <c r="F59" s="1">
+      <c r="F59" s="4">
         <v>4.3</v>
       </c>
       <c r="G59">
@@ -3447,7 +3483,7 @@
       </c>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="2">
+      <c r="A60" s="3">
         <v>43327</v>
       </c>
       <c r="B60">
@@ -3464,7 +3500,7 @@
         <f t="shared" si="4"/>
         <v>299.852777777778</v>
       </c>
-      <c r="F60" s="1">
+      <c r="F60" s="4">
         <v>3.4</v>
       </c>
       <c r="G60">
@@ -3476,7 +3512,7 @@
       </c>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="2">
+      <c r="A61" s="3">
         <v>43331</v>
       </c>
       <c r="B61">
@@ -3493,11 +3529,11 @@
         <f t="shared" si="4"/>
         <v>303.822222222222</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F61" s="4">
         <v>4</v>
       </c>
       <c r="G61">
-        <f>E61-5.366*56</f>
+        <f t="shared" ref="G61:G63" si="18">E61-5.366*56</f>
         <v>3.32622222222221</v>
       </c>
       <c r="H61">
@@ -3505,6 +3541,154 @@
       </c>
       <c r="I61" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="3">
+        <v>43333</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="14"/>
+        <v>305</v>
+      </c>
+      <c r="C62">
+        <v>20</v>
+      </c>
+      <c r="D62">
+        <v>26</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="4"/>
+        <v>305.851388888889</v>
+      </c>
+      <c r="F62" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="18"/>
+        <v>5.35538888888891</v>
+      </c>
+      <c r="I62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="3">
+        <v>43335</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="14"/>
+        <v>307</v>
+      </c>
+      <c r="C63">
+        <v>20</v>
+      </c>
+      <c r="D63">
+        <v>31</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="4"/>
+        <v>307.854861111111</v>
+      </c>
+      <c r="F63" s="4">
+        <v>4.4</v>
+      </c>
+      <c r="G63">
+        <f>E63-5.366*57</f>
+        <v>1.99286111111115</v>
+      </c>
+      <c r="H63">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="3">
+        <v>43339</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="14"/>
+        <v>311</v>
+      </c>
+      <c r="C64">
+        <v>20</v>
+      </c>
+      <c r="D64">
+        <v>22</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="4"/>
+        <v>311.848611111111</v>
+      </c>
+      <c r="F64" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="G64">
+        <f t="shared" ref="G64:G66" si="19">E64-5.366*58</f>
+        <v>0.620611111111032</v>
+      </c>
+      <c r="H64">
+        <v>58</v>
+      </c>
+      <c r="I64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="3">
+        <v>43340</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="14"/>
+        <v>312</v>
+      </c>
+      <c r="C65">
+        <v>20</v>
+      </c>
+      <c r="D65">
+        <v>36</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="4"/>
+        <v>312.858333333333</v>
+      </c>
+      <c r="F65" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="19"/>
+        <v>1.63033333333306</v>
+      </c>
+      <c r="I65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="3">
+        <v>43341</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="14"/>
+        <v>313</v>
+      </c>
+      <c r="C66">
+        <v>21</v>
+      </c>
+      <c r="D66">
+        <v>19</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="4"/>
+        <v>313.888194444444</v>
+      </c>
+      <c r="F66" s="4">
+        <v>4</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="19"/>
+        <v>2.66019444444447</v>
+      </c>
+      <c r="I66" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3518,14 +3702,111 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="6"/>
+  <cols>
+    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="4" max="4" width="5.75" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="3">
+        <v>43327</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>28</v>
+      </c>
+      <c r="E2">
+        <f>(B2*1440+C2*60+D2)/1440</f>
+        <v>0.852777777777778</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3">
+        <v>43331</v>
+      </c>
+      <c r="B3">
+        <f>A3-A2+B2</f>
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>44</v>
+      </c>
+      <c r="E3">
+        <f>(B3*1440+C3*60+D3)/1440</f>
+        <v>4.82222222222222</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3">
+        <v>43339</v>
+      </c>
+      <c r="B4">
+        <f>A4-A3+B3</f>
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <f>(B4*1440+C4*60+D4)/1440</f>
+        <v>12.8486111111111</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3.6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Add data for stars
</commit_message>
<xml_diff>
--- a/delta_cep/delta_cep.xlsx
+++ b/delta_cep/delta_cep.xlsx
@@ -62,10 +62,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.0_ "/>
   </numFmts>
   <fonts count="21">
@@ -84,9 +84,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -152,9 +151,40 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -174,13 +204,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -191,29 +214,6 @@
     <font>
       <b/>
       <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -309,6 +309,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -339,24 +369,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -382,18 +394,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,6 +447,50 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -470,30 +514,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -508,26 +528,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -560,115 +560,115 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1192,10 +1192,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>delta_cep!$G$46:$G$70</c:f>
+              <c:f>delta_cep!$G$46:$G$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>4.61736111111117</c:v>
                 </c:pt>
@@ -1270,16 +1270,22 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>1.8705555555556</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.87333333333333</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.74061111111109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>delta_cep!$F$46:$F$70</c:f>
+              <c:f>delta_cep!$F$46:$F$72</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>3.4</c:v>
                 </c:pt>
@@ -1353,6 +1359,12 @@
                   <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -1899,10 +1911,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2244,7 +2256,7 @@
         <v>9</v>
       </c>
       <c r="E13">
-        <f t="shared" ref="E13:E70" si="4">(B13*1440+C13*60+D13)/1440</f>
+        <f t="shared" ref="E13:E72" si="4">(B13*1440+C13*60+D13)/1440</f>
         <v>12.88125</v>
       </c>
       <c r="F13" s="4">
@@ -3099,7 +3111,7 @@
         <v>43300</v>
       </c>
       <c r="B46">
-        <f t="shared" ref="B46:B70" si="14">A46-A45+B45</f>
+        <f t="shared" ref="B46:B72" si="14">A46-A45+B45</f>
         <v>272</v>
       </c>
       <c r="C46">
@@ -3827,7 +3839,7 @@
         <v>4</v>
       </c>
       <c r="G70">
-        <f>E70-5.366*60</f>
+        <f t="shared" ref="G70:G72" si="21">E70-5.366*60</f>
         <v>1.8705555555556</v>
       </c>
       <c r="H70">
@@ -3835,6 +3847,64 @@
       </c>
       <c r="I70" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="3">
+        <v>43352</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="14"/>
+        <v>324</v>
+      </c>
+      <c r="C71">
+        <v>20</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="4"/>
+        <v>324.833333333333</v>
+      </c>
+      <c r="F71" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="21"/>
+        <v>2.87333333333333</v>
+      </c>
+      <c r="I71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="3">
+        <v>43367</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="14"/>
+        <v>339</v>
+      </c>
+      <c r="C72">
+        <v>19</v>
+      </c>
+      <c r="D72">
+        <v>10</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="4"/>
+        <v>339.798611111111</v>
+      </c>
+      <c r="F72" s="4">
+        <v>4</v>
+      </c>
+      <c r="G72">
+        <f>E72-5.366*63</f>
+        <v>1.74061111111109</v>
+      </c>
+      <c r="I72" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3848,13 +3918,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="6"/>
   <cols>
     <col min="3" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="5.75" customWidth="1"/>
@@ -3898,7 +3968,7 @@
         <v>28</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E7" si="0">(B2*1440+C2*60+D2)/1440</f>
+        <f t="shared" ref="E2:E8" si="0">(B2*1440+C2*60+D2)/1440</f>
         <v>0.852777777777778</v>
       </c>
       <c r="F2" s="1">
@@ -3913,7 +3983,7 @@
         <v>43331</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B7" si="1">A3-A2+B2</f>
+        <f t="shared" ref="B3:B8" si="1">A3-A2+B2</f>
         <v>4</v>
       </c>
       <c r="C3">
@@ -4016,6 +4086,28 @@
       </c>
       <c r="F7" s="1">
         <v>3.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3">
+        <v>43367</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>40.7986111111111</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Vstar data of Delta Cep
</commit_message>
<xml_diff>
--- a/delta_cep/delta_cep.xlsx
+++ b/delta_cep/delta_cep.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21045" windowHeight="10350"/>
+    <workbookView windowWidth="21045" windowHeight="10080"/>
   </bookViews>
   <sheets>
     <sheet name="delta_cep" sheetId="1" r:id="rId1"/>
@@ -78,13 +78,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -152,9 +145,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,14 +207,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,13 +237,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -261,13 +267,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -279,19 +351,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,121 +417,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,21 +451,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -520,6 +505,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -533,148 +533,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1192,10 +1192,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>delta_cep!$G$46:$G$106</c:f>
+              <c:f>delta_cep!$G$46:$G$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="61"/>
+                <c:ptCount val="63"/>
                 <c:pt idx="0">
                   <c:v>4.61736111111117</c:v>
                 </c:pt>
@@ -1378,16 +1378,22 @@
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>4.1998333333334</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.77333333333337</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.389972222222241</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>delta_cep!$F$46:$F$106</c:f>
+              <c:f>delta_cep!$F$46:$F$108</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="61"/>
+                <c:ptCount val="63"/>
                 <c:pt idx="0">
                   <c:v>3.4</c:v>
                 </c:pt>
@@ -1570,6 +1576,12 @@
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2115,10 +2127,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J106"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3315,7 +3327,7 @@
         <v>43300</v>
       </c>
       <c r="B46">
-        <f t="shared" ref="B46:B106" si="14">A46-A45+B45</f>
+        <f t="shared" ref="B46:B108" si="14">A46-A45+B45</f>
         <v>272</v>
       </c>
       <c r="C46">
@@ -4242,7 +4254,7 @@
         <v>26</v>
       </c>
       <c r="E77">
-        <f t="shared" ref="E77:E105" si="24">(B77*1440+C77*60+D77)/1440</f>
+        <f t="shared" ref="E77:E108" si="24">(B77*1440+C77*60+D77)/1440</f>
         <v>349.809722222222</v>
       </c>
       <c r="F77" s="4">
@@ -5049,7 +5061,7 @@
         <v>3.8</v>
       </c>
       <c r="G105">
-        <f>E105-5.366*81</f>
+        <f t="shared" ref="G105:G107" si="34">E105-5.366*81</f>
         <v>1.19775000000004</v>
       </c>
       <c r="H105">
@@ -5074,14 +5086,14 @@
         <v>18</v>
       </c>
       <c r="E106">
-        <f>(B106*1440+C106*60+D106)/1440</f>
+        <f t="shared" si="24"/>
         <v>438.845833333333</v>
       </c>
       <c r="F106" s="4">
         <v>3.3</v>
       </c>
       <c r="G106">
-        <f>E106-5.366*81</f>
+        <f t="shared" si="34"/>
         <v>4.1998333333334</v>
       </c>
       <c r="I106" t="s">
@@ -5089,6 +5101,58 @@
       </c>
       <c r="J106">
         <v>2019</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" s="3">
+        <v>43485</v>
+      </c>
+      <c r="B107">
+        <f t="shared" si="14"/>
+        <v>457</v>
+      </c>
+      <c r="C107">
+        <v>21</v>
+      </c>
+      <c r="D107">
+        <v>12</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="24"/>
+        <v>457.883333333333</v>
+      </c>
+      <c r="F107" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="G107">
+        <f>E107-5.366*85</f>
+        <v>1.77333333333337</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" s="3">
+        <v>43489</v>
+      </c>
+      <c r="B108">
+        <f t="shared" si="14"/>
+        <v>461</v>
+      </c>
+      <c r="C108">
+        <v>20</v>
+      </c>
+      <c r="D108">
+        <v>47</v>
+      </c>
+      <c r="E108">
+        <f t="shared" si="24"/>
+        <v>461.865972222222</v>
+      </c>
+      <c r="F108" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="G108">
+        <f>E108-5.366*86</f>
+        <v>0.389972222222241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for delta_Cep
</commit_message>
<xml_diff>
--- a/delta_cep/delta_cep.xlsx
+++ b/delta_cep/delta_cep.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21045" windowHeight="10080"/>
+    <workbookView windowWidth="21600" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="delta_cep" sheetId="1" r:id="rId1"/>
-    <sheet name="mu_cep" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="delta_cep_2019" sheetId="3" r:id="rId2"/>
+    <sheet name="mu_cep" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="13">
   <si>
     <t>日期</t>
   </si>
@@ -63,9 +63,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.0_ "/>
   </numFmts>
   <fonts count="21">
@@ -78,15 +78,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -114,9 +113,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -130,14 +128,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -145,16 +135,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -168,9 +151,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -199,6 +181,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
@@ -206,15 +204,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -222,7 +214,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,7 +237,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -249,25 +261,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,25 +279,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,13 +315,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -369,55 +369,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,17 +431,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -456,16 +450,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -487,17 +481,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -506,25 +489,42 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -536,10 +536,10 @@
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -548,31 +548,31 @@
     <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -581,100 +581,100 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1192,10 +1192,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>delta_cep!$G$46:$G$108</c:f>
+              <c:f>delta_cep!$G$46:$G$105</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="63"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>4.61736111111117</c:v>
                 </c:pt>
@@ -1375,25 +1375,16 @@
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>1.19775000000004</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>4.1998333333334</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>1.77333333333337</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.389972222222241</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>delta_cep!$F$46:$F$108</c:f>
+              <c:f>delta_cep!$F$46:$F$105</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="63"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>3.4</c:v>
                 </c:pt>
@@ -1574,14 +1565,121 @@
                 <c:pt idx="59">
                   <c:v>3.8</c:v>
                 </c:pt>
-                <c:pt idx="60">
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>"2019"</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>delta_cep_2019!$G$2:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4.1998333333334</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.77333333333337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.389972222222241</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.28788888888891</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.32747222222224</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.34508333333338</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.07283333333339</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00538888888900146</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99358333333339</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.99636111111124</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.97552777777787</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.54911111111119</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>delta_cep_2019!$F$2:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.0_ </c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
                   <c:v>3.3</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="1">
                   <c:v>3.9</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="2">
                   <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1811,14 +1909,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>635</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>302260</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>84455</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>85090</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1826,7 +1924,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5210175" y="171450"/>
+        <a:off x="5210175" y="635"/>
         <a:ext cx="8941435" cy="5742305"/>
       </xdr:xfrm>
       <a:graphic>
@@ -2127,10 +2225,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J108"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3327,7 +3425,7 @@
         <v>43300</v>
       </c>
       <c r="B46">
-        <f t="shared" ref="B46:B108" si="14">A46-A45+B45</f>
+        <f t="shared" ref="B46:B109" si="14">A46-A45+B45</f>
         <v>272</v>
       </c>
       <c r="C46">
@@ -4254,7 +4352,7 @@
         <v>26</v>
       </c>
       <c r="E77">
-        <f t="shared" ref="E77:E108" si="24">(B77*1440+C77*60+D77)/1440</f>
+        <f t="shared" ref="E77:E110" si="24">(B77*1440+C77*60+D77)/1440</f>
         <v>349.809722222222</v>
       </c>
       <c r="F77" s="4">
@@ -5071,89 +5169,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
-      <c r="A106" s="3">
-        <v>43466</v>
-      </c>
-      <c r="B106">
-        <f t="shared" si="14"/>
-        <v>438</v>
-      </c>
-      <c r="C106">
-        <v>20</v>
-      </c>
-      <c r="D106">
-        <v>18</v>
-      </c>
-      <c r="E106">
-        <f t="shared" si="24"/>
-        <v>438.845833333333</v>
-      </c>
-      <c r="F106" s="4">
-        <v>3.3</v>
-      </c>
-      <c r="G106">
-        <f t="shared" si="34"/>
-        <v>4.1998333333334</v>
-      </c>
-      <c r="I106" t="s">
-        <v>12</v>
-      </c>
-      <c r="J106">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7">
-      <c r="A107" s="3">
-        <v>43485</v>
-      </c>
-      <c r="B107">
-        <f t="shared" si="14"/>
-        <v>457</v>
-      </c>
-      <c r="C107">
-        <v>21</v>
-      </c>
-      <c r="D107">
-        <v>12</v>
-      </c>
-      <c r="E107">
-        <f t="shared" si="24"/>
-        <v>457.883333333333</v>
-      </c>
-      <c r="F107" s="4">
-        <v>3.9</v>
-      </c>
-      <c r="G107">
-        <f>E107-5.366*85</f>
-        <v>1.77333333333337</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7">
-      <c r="A108" s="3">
-        <v>43489</v>
-      </c>
-      <c r="B108">
-        <f t="shared" si="14"/>
-        <v>461</v>
-      </c>
-      <c r="C108">
-        <v>20</v>
-      </c>
-      <c r="D108">
-        <v>47</v>
-      </c>
-      <c r="E108">
-        <f t="shared" si="24"/>
-        <v>461.865972222222</v>
-      </c>
-      <c r="F108" s="4">
-        <v>3.8</v>
-      </c>
-      <c r="G108">
-        <f>E108-5.366*86</f>
-        <v>0.389972222222241</v>
-      </c>
+    <row r="106" spans="1:1">
+      <c r="A106" s="3"/>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="3"/>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="3"/>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="3"/>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5166,10 +5195,413 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="7" max="7" width="12.625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="3">
+        <v>43466</v>
+      </c>
+      <c r="B2">
+        <f>A2-delta_cep!A2+delta_cep!B2</f>
+        <v>438</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E13" si="0">(B2*1440+C2*60+D2)/1440</f>
+        <v>438.845833333333</v>
+      </c>
+      <c r="F2" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="G2">
+        <f>E2-5.366*81</f>
+        <v>4.1998333333334</v>
+      </c>
+      <c r="H2">
+        <v>81</v>
+      </c>
+      <c r="I2">
+        <v>2019</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3">
+        <v>43485</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B13" si="1">A3-A2+B2</f>
+        <v>457</v>
+      </c>
+      <c r="C3">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>457.883333333333</v>
+      </c>
+      <c r="F3" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="G3">
+        <f>E3-5.366*85</f>
+        <v>1.77333333333337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3">
+        <v>43489</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="1"/>
+        <v>461</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>47</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>461.865972222222</v>
+      </c>
+      <c r="F4" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G7" si="2">E4-5.366*86</f>
+        <v>0.389972222222241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3">
+        <v>43491</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>463</v>
+      </c>
+      <c r="C5">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>463.763888888889</v>
+      </c>
+      <c r="F5" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>2.28788888888891</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3">
+        <v>43492</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>464</v>
+      </c>
+      <c r="C6">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>464.803472222222</v>
+      </c>
+      <c r="F6" s="4">
+        <v>4.1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>3.32747222222224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="3">
+        <v>43714</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>686</v>
+      </c>
+      <c r="C7">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>51</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>686.827083333333</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="G7">
+        <f>E7-5.366*127</f>
+        <v>5.34508333333338</v>
+      </c>
+      <c r="H7">
+        <v>127</v>
+      </c>
+      <c r="J7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3">
+        <v>43715</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>687</v>
+      </c>
+      <c r="C8">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>687.920833333333</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="G8">
+        <f>E8-5.366*128</f>
+        <v>1.07283333333339</v>
+      </c>
+      <c r="H8">
+        <v>128</v>
+      </c>
+      <c r="J8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="3">
+        <v>43730</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>702</v>
+      </c>
+      <c r="C9">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>50</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>702.951388888889</v>
+      </c>
+      <c r="F9" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9:G13" si="3">E9-5.366*131</f>
+        <v>0.00538888888900146</v>
+      </c>
+      <c r="H9">
+        <v>131</v>
+      </c>
+      <c r="J9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="3">
+        <v>43731</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>703</v>
+      </c>
+      <c r="C10">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>33</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>703.939583333333</v>
+      </c>
+      <c r="F10" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>0.99358333333339</v>
+      </c>
+      <c r="J10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="3">
+        <v>43734</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>706</v>
+      </c>
+      <c r="C11">
+        <v>22</v>
+      </c>
+      <c r="D11">
+        <v>37</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>706.942361111111</v>
+      </c>
+      <c r="F11" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>3.99636111111124</v>
+      </c>
+      <c r="J11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="3">
+        <v>43735</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>707</v>
+      </c>
+      <c r="C12">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>707.921527777778</v>
+      </c>
+      <c r="F12" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>4.97552777777787</v>
+      </c>
+      <c r="J12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="3">
+        <v>43737</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>709</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>40</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>709.861111111111</v>
+      </c>
+      <c r="F13" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="G13">
+        <f>E13-5.366*132</f>
+        <v>1.54911111111119</v>
+      </c>
+      <c r="H13">
+        <v>132</v>
+      </c>
+      <c r="J13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -5218,14 +5650,14 @@
         <v>28</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E25" si="0">(B2*1440+C2*60+D2)/1440</f>
+        <f t="shared" ref="E2:E27" si="0">(B2*1440+C2*60+D2)/1440</f>
         <v>0.852777777777778</v>
       </c>
       <c r="F2" s="1">
         <v>3.5</v>
       </c>
       <c r="G2">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -5233,7 +5665,7 @@
         <v>43331</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B25" si="1">A3-A2+B2</f>
+        <f t="shared" ref="B3:B27" si="1">A3-A2+B2</f>
         <v>4</v>
       </c>
       <c r="C3">
@@ -5732,26 +6164,57 @@
       </c>
       <c r="F25" s="1">
         <v>3.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="3">
+        <v>43491</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>164</v>
+      </c>
+      <c r="C26">
+        <v>18</v>
+      </c>
+      <c r="D26">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>164.763888888889</v>
+      </c>
+      <c r="F26" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="G26">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="3">
+        <v>43730</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="1"/>
+        <v>403</v>
+      </c>
+      <c r="C27">
+        <v>22</v>
+      </c>
+      <c r="D27">
+        <v>50</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>403.951388888889</v>
+      </c>
+      <c r="F27" s="1">
+        <v>3.6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add data of year 2020.
</commit_message>
<xml_diff>
--- a/delta_cep/delta_cep.xlsx
+++ b/delta_cep/delta_cep.xlsx
@@ -9,14 +9,15 @@
   <sheets>
     <sheet name="delta_cep" sheetId="1" r:id="rId1"/>
     <sheet name="delta_cep_2019" sheetId="3" r:id="rId2"/>
-    <sheet name="mu_cep" sheetId="2" r:id="rId3"/>
+    <sheet name="delta_cep_2020" sheetId="4" r:id="rId3"/>
+    <sheet name="mu_cep" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="13">
   <si>
     <t>日期</t>
   </si>
@@ -62,10 +63,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.0_ "/>
   </numFmts>
   <fonts count="21">
@@ -77,29 +78,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -108,43 +88,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -159,7 +102,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -170,6 +128,52 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -189,9 +193,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -199,30 +224,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,7 +238,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,25 +286,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -328,12 +371,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -385,42 +422,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -428,21 +429,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -471,6 +457,56 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -493,188 +529,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1596,10 +1597,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>delta_cep_2019!$G$2:$G$48</c:f>
+              <c:f>delta_cep_2019!$G$2:$G$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="47"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>4.1998333333334</c:v>
                 </c:pt>
@@ -1740,16 +1741,31 @@
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>4.79458333333343</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.34455555555564</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.36886111111119</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.10008333333337</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.70630555555567</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.34516666666673</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>delta_cep_2019!$F$2:$F$48</c:f>
+              <c:f>delta_cep_2019!$F$2:$F$53</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="47"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>3.3</c:v>
                 </c:pt>
@@ -1890,6 +1906,75 @@
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>"2020"</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>delta_cep_2020!$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.23058333333336</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>delta_cep_2020!$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.0_ </c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2437,8 +2522,8 @@
   <sheetPr/>
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -5405,10 +5490,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -5461,7 +5546,7 @@
         <v>18</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E48" si="0">(B2*1440+C2*60+D2)/1440</f>
+        <f t="shared" ref="E2:E53" si="0">(B2*1440+C2*60+D2)/1440</f>
         <v>438.845833333333</v>
       </c>
       <c r="F2" s="4">
@@ -5486,7 +5571,7 @@
         <v>43485</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B48" si="1">A3-A2+B2</f>
+        <f t="shared" ref="B3:B53" si="1">A3-A2+B2</f>
         <v>457</v>
       </c>
       <c r="C3">
@@ -6804,7 +6889,7 @@
         <v>3.8</v>
       </c>
       <c r="G46">
-        <f t="shared" ref="G46:G48" si="15">E46-5.366*145</f>
+        <f t="shared" ref="G46:G49" si="15">E46-5.366*145</f>
         <v>0.690416666666692</v>
       </c>
       <c r="H46">
@@ -6867,6 +6952,151 @@
       </c>
       <c r="H48">
         <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="3">
+        <v>43812</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="1"/>
+        <v>784</v>
+      </c>
+      <c r="C49">
+        <v>18</v>
+      </c>
+      <c r="D49">
+        <v>44</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>784.780555555556</v>
+      </c>
+      <c r="F49" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="G49">
+        <f t="shared" ref="G49:G51" si="16">E49-5.366*146</f>
+        <v>1.34455555555564</v>
+      </c>
+      <c r="H49">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="3">
+        <v>43815</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="1"/>
+        <v>787</v>
+      </c>
+      <c r="C50">
+        <v>19</v>
+      </c>
+      <c r="D50">
+        <v>19</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>787.804861111111</v>
+      </c>
+      <c r="F50" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="16"/>
+        <v>4.36886111111119</v>
+      </c>
+      <c r="H50">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="3">
+        <v>43818</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="1"/>
+        <v>790</v>
+      </c>
+      <c r="C51">
+        <v>21</v>
+      </c>
+      <c r="D51">
+        <v>39</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>790.902083333333</v>
+      </c>
+      <c r="F51" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="G51">
+        <f>E51-5.366*147</f>
+        <v>2.10008333333337</v>
+      </c>
+      <c r="H51">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="3">
+        <v>43826</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="1"/>
+        <v>798</v>
+      </c>
+      <c r="C52">
+        <v>20</v>
+      </c>
+      <c r="D52">
+        <v>59</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>798.874305555556</v>
+      </c>
+      <c r="F52" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="G52">
+        <f>E52-5.366*148</f>
+        <v>4.70630555555567</v>
+      </c>
+      <c r="H52">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="3">
+        <v>43830</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="1"/>
+        <v>802</v>
+      </c>
+      <c r="C53">
+        <v>21</v>
+      </c>
+      <c r="D53">
+        <v>6</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>802.879166666667</v>
+      </c>
+      <c r="F53" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="G53">
+        <f>E53-5.366*149</f>
+        <v>3.34516666666673</v>
+      </c>
+      <c r="H53">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -6876,6 +7106,97 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <cols>
+    <col min="2" max="2" width="8.875" customWidth="1"/>
+    <col min="3" max="3" width="4.375" customWidth="1"/>
+    <col min="4" max="4" width="4.625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="5.875" customWidth="1"/>
+    <col min="7" max="7" width="12.625"/>
+    <col min="8" max="8" width="7.125" customWidth="1"/>
+    <col min="9" max="9" width="7.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="3">
+        <v>43831</v>
+      </c>
+      <c r="B2">
+        <f>A2-delta_cep!A2+delta_cep!B2</f>
+        <v>803</v>
+      </c>
+      <c r="C2">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <f>(B2*1440+C2*60+D2)/1440</f>
+        <v>803.764583333333</v>
+      </c>
+      <c r="F2" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="G2">
+        <f>E2-5.366*H2</f>
+        <v>4.23058333333336</v>
+      </c>
+      <c r="H2">
+        <v>149</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:G29"/>

</xml_diff>

<commit_message>
Add data from 2020 Aug
</commit_message>
<xml_diff>
--- a/delta_cep/delta_cep.xlsx
+++ b/delta_cep/delta_cep.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20925" windowHeight="10155" activeTab="3"/>
+    <workbookView windowWidth="20925" windowHeight="9885"/>
   </bookViews>
   <sheets>
     <sheet name="delta_cep" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="14">
   <si>
     <t>日期</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>w</t>
+  </si>
+  <si>
+    <t>02</t>
   </si>
 </sst>
 </file>
@@ -207,8 +210,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,9 +225,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,7 +241,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,55 +271,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,19 +301,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,6 +325,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -364,37 +361,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,13 +379,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,10 +540,10 @@
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -549,16 +552,16 @@
     <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -570,10 +573,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -594,25 +597,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -624,62 +627,62 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -693,6 +696,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1957,10 +1963,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>delta_cep_2020!$G$2:$G$9</c:f>
+              <c:f>delta_cep_2020!$G$2:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>4.23058333333336</c:v>
                 </c:pt>
@@ -1984,16 +1990,34 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.311611111111119</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.587944444444474</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.01205555555566</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.98844444444444</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.99052777777774</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.702999999999975</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.59397222222219</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>delta_cep_2020!$F$2:$F$9</c:f>
+              <c:f>delta_cep_2020!$F$2:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>3.4</c:v>
                 </c:pt>
@@ -2017,6 +2041,24 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2564,8 +2606,8 @@
   <sheetPr/>
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -7150,10 +7192,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -7209,14 +7251,14 @@
         <v>21</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E9" si="0">(B2*1440+C2*60+D2)/1440</f>
+        <f t="shared" ref="E2:E16" si="0">(B2*1440+C2*60+D2)/1440</f>
         <v>803.764583333333</v>
       </c>
       <c r="F2" s="4">
         <v>3.4</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G9" si="1">E2-5.366*H2</f>
+        <f t="shared" ref="G2:G10" si="1">E2-5.366*H2</f>
         <v>4.23058333333336</v>
       </c>
       <c r="H2">
@@ -7430,6 +7472,180 @@
       </c>
       <c r="H9">
         <v>157</v>
+      </c>
+    </row>
+    <row r="10" customFormat="1" spans="1:8">
+      <c r="A10" s="3">
+        <v>43881</v>
+      </c>
+      <c r="B10">
+        <f>A10-delta_cep!A10+delta_cep!B10</f>
+        <v>853</v>
+      </c>
+      <c r="C10">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>46</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>853.781944444444</v>
+      </c>
+      <c r="F10" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="G10">
+        <f>E10-5.366*H10</f>
+        <v>0.587944444444474</v>
+      </c>
+      <c r="H10">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" customFormat="1" spans="1:8">
+      <c r="A11" s="3">
+        <v>44055</v>
+      </c>
+      <c r="B11">
+        <f>A11-delta_cep!A12+delta_cep!B12</f>
+        <v>1027</v>
+      </c>
+      <c r="C11">
+        <v>22</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <f>(B11*1440+C11*60+D11)/1440</f>
+        <v>1027.91805555556</v>
+      </c>
+      <c r="F11" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="G11">
+        <f>E11-5.366*H11</f>
+        <v>3.01205555555566</v>
+      </c>
+      <c r="H11">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" customFormat="1" spans="1:8">
+      <c r="A12" s="3">
+        <v>44056</v>
+      </c>
+      <c r="B12">
+        <f>A12-delta_cep!A13+delta_cep!B13</f>
+        <v>1028</v>
+      </c>
+      <c r="C12">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>28</v>
+      </c>
+      <c r="E12">
+        <f>(B12*1440+C12*60+D12)/1440</f>
+        <v>1028.89444444444</v>
+      </c>
+      <c r="F12" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="G12">
+        <f>E12-5.366*H12</f>
+        <v>3.98844444444444</v>
+      </c>
+      <c r="H12">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" customFormat="1" spans="1:8">
+      <c r="A13" s="3">
+        <v>44057</v>
+      </c>
+      <c r="B13">
+        <f>A13-delta_cep!A14+delta_cep!B14</f>
+        <v>1029</v>
+      </c>
+      <c r="C13">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>31</v>
+      </c>
+      <c r="E13">
+        <f>(B13*1440+C13*60+D13)/1440</f>
+        <v>1029.89652777778</v>
+      </c>
+      <c r="F13" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="G13">
+        <f>E13-5.366*H13</f>
+        <v>4.99052777777774</v>
+      </c>
+      <c r="H13">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" customFormat="1" spans="1:8">
+      <c r="A14" s="3">
+        <v>44058</v>
+      </c>
+      <c r="B14">
+        <f>A14-delta_cep!A15+delta_cep!B15</f>
+        <v>1030</v>
+      </c>
+      <c r="C14">
+        <v>23</v>
+      </c>
+      <c r="D14">
+        <v>24</v>
+      </c>
+      <c r="E14">
+        <f>(B14*1440+C14*60+D14)/1440</f>
+        <v>1030.975</v>
+      </c>
+      <c r="F14" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="G14">
+        <f>E14-5.366*H14</f>
+        <v>0.702999999999975</v>
+      </c>
+      <c r="H14">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" customFormat="1" spans="1:8">
+      <c r="A15" s="3">
+        <v>44059</v>
+      </c>
+      <c r="B15">
+        <f>A15-delta_cep!A16+delta_cep!B16</f>
+        <v>1031</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>47</v>
+      </c>
+      <c r="E15">
+        <f>(B15*1440+C15*60+D15)/1440</f>
+        <v>1031.86597222222</v>
+      </c>
+      <c r="F15" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="G15">
+        <f>E15-5.366*H15</f>
+        <v>1.59397222222219</v>
+      </c>
+      <c r="H15">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -7443,7 +7659,7 @@
   <sheetPr/>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add data until 2020/10/7
</commit_message>
<xml_diff>
--- a/delta_cep/delta_cep.xlsx
+++ b/delta_cep/delta_cep.xlsx
@@ -67,9 +67,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.0_ "/>
   </numFmts>
   <fonts count="21">
@@ -1963,10 +1963,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>delta_cep_2020!$G$2:$G$33</c:f>
+              <c:f>delta_cep_2020!$G$2:$G$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>4.23058333333336</c:v>
                 </c:pt>
@@ -2062,16 +2062,28 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>3.43686111111128</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.05836111111125</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.02572222222238</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.310388888888838</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.36455555555563</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>delta_cep_2020!$F$2:$F$33</c:f>
+              <c:f>delta_cep_2020!$F$2:$F$37</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>3.4</c:v>
                 </c:pt>
@@ -2167,6 +2179,18 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2714,8 +2738,8 @@
   <sheetPr/>
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -5684,7 +5708,7 @@
   <sheetPr/>
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
@@ -7300,10 +7324,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -7359,14 +7383,14 @@
         <v>21</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E33" si="0">(B2*1440+C2*60+D2)/1440</f>
+        <f t="shared" ref="E2:E37" si="0">(B2*1440+C2*60+D2)/1440</f>
         <v>803.764583333333</v>
       </c>
       <c r="F2" s="4">
         <v>3.4</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G33" si="1">E2-5.366*H2</f>
+        <f t="shared" ref="G2:G37" si="1">E2-5.366*H2</f>
         <v>4.23058333333336</v>
       </c>
       <c r="H2">
@@ -8276,6 +8300,122 @@
       </c>
       <c r="H33">
         <v>198</v>
+      </c>
+    </row>
+    <row r="34" customFormat="1" spans="1:8">
+      <c r="A34" s="3">
+        <v>44098</v>
+      </c>
+      <c r="B34">
+        <f>A34-delta_cep!A35+delta_cep!B35</f>
+        <v>1070</v>
+      </c>
+      <c r="C34">
+        <v>21</v>
+      </c>
+      <c r="D34">
+        <v>25</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>1070.89236111111</v>
+      </c>
+      <c r="F34" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>3.05836111111125</v>
+      </c>
+      <c r="H34">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" customFormat="1" spans="1:8">
+      <c r="A35" s="3">
+        <v>44100</v>
+      </c>
+      <c r="B35">
+        <f>A35-delta_cep!A36+delta_cep!B36</f>
+        <v>1072</v>
+      </c>
+      <c r="C35">
+        <v>20</v>
+      </c>
+      <c r="D35">
+        <v>38</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>1072.85972222222</v>
+      </c>
+      <c r="F35" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>5.02572222222238</v>
+      </c>
+      <c r="H35">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" customFormat="1" spans="1:8">
+      <c r="A36" s="3">
+        <v>44106</v>
+      </c>
+      <c r="B36">
+        <f>A36-delta_cep!A37+delta_cep!B37</f>
+        <v>1078</v>
+      </c>
+      <c r="C36">
+        <v>21</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>1078.87638888889</v>
+      </c>
+      <c r="F36" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>0.310388888888838</v>
+      </c>
+      <c r="H36">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" customFormat="1" spans="1:8">
+      <c r="A37" s="3">
+        <v>44111</v>
+      </c>
+      <c r="B37">
+        <f>A37-delta_cep!A38+delta_cep!B38</f>
+        <v>1083</v>
+      </c>
+      <c r="C37">
+        <v>22</v>
+      </c>
+      <c r="D37">
+        <v>20</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>1083.93055555556</v>
+      </c>
+      <c r="F37" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>5.36455555555563</v>
+      </c>
+      <c r="H37">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -8290,7 +8430,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>

</xml_diff>

<commit_message>
Add data until 2021/8/4
</commit_message>
<xml_diff>
--- a/delta_cep/delta_cep.xlsx
+++ b/delta_cep/delta_cep.xlsx
@@ -69,9 +69,9 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.0_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -83,7 +83,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -91,14 +91,80 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -112,8 +178,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -128,45 +195,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -182,30 +211,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,14 +220,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -242,7 +242,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -254,37 +410,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,133 +422,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,80 +433,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -533,153 +459,227 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2428,10 +2428,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>delta_cep_2021!$G$2:$G$5</c:f>
+              <c:f>delta_cep_2021!$G$2:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.08075000000008</c:v>
                 </c:pt>
@@ -2443,16 +2443,37 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.91538888888886</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.08122222222232</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.08330555555563</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.74647222222234</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.85975000000008</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.96100000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.5706944444446</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.458805555555728</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>delta_cep_2021!$F$2:$F$5</c:f>
+              <c:f>delta_cep_2021!$F$2:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>3.5</c:v>
                 </c:pt>
@@ -2464,6 +2485,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3012,7 +3054,7 @@
   <dimension ref="A1:I110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -9687,13 +9729,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="9.5" customWidth="1"/>
   </cols>
@@ -9739,14 +9781,14 @@
         <v>51</v>
       </c>
       <c r="E2">
-        <f>(B2*1440+C2*60+D2)/1440</f>
+        <f t="shared" ref="E2:E12" si="0">(B2*1440+C2*60+D2)/1440</f>
         <v>1169.86875</v>
       </c>
       <c r="F2" s="4">
         <v>3.5</v>
       </c>
       <c r="G2">
-        <f>E2-5.366*H2</f>
+        <f t="shared" ref="G2:G12" si="1">E2-5.366*H2</f>
         <v>0.08075000000008</v>
       </c>
       <c r="H2">
@@ -9768,14 +9810,14 @@
         <v>26</v>
       </c>
       <c r="E3">
-        <f>(B3*1440+C3*60+D3)/1440</f>
+        <f t="shared" si="0"/>
         <v>1185.85138888889</v>
       </c>
       <c r="F3" s="4">
         <v>3.6</v>
       </c>
       <c r="G3">
-        <f>E3-5.366*H3</f>
+        <f t="shared" si="1"/>
         <v>5.3313888888888</v>
       </c>
       <c r="H3">
@@ -9797,14 +9839,14 @@
         <v>36</v>
       </c>
       <c r="E4">
-        <f>(B4*1440+C4*60+D4)/1440</f>
+        <f t="shared" si="0"/>
         <v>1186.85833333333</v>
       </c>
       <c r="F4" s="4">
         <v>3.9</v>
       </c>
       <c r="G4">
-        <f>E4-5.366*H4</f>
+        <f t="shared" si="1"/>
         <v>0.972333333333381</v>
       </c>
       <c r="H4">
@@ -9826,18 +9868,221 @@
         <v>14</v>
       </c>
       <c r="E5">
-        <f>(B5*1440+C5*60+D5)/1440</f>
+        <f t="shared" si="0"/>
         <v>1187.80138888889</v>
       </c>
       <c r="F5" s="4">
         <v>3.8</v>
       </c>
       <c r="G5">
-        <f>E5-5.366*H5</f>
+        <f t="shared" si="1"/>
         <v>1.91538888888886</v>
       </c>
       <c r="H5">
         <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="3">
+        <v>44244</v>
+      </c>
+      <c r="B6">
+        <f>A6-delta_cep!A6+delta_cep!B6</f>
+        <v>1216</v>
+      </c>
+      <c r="C6">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1216.79722222222</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>4.08122222222232</v>
+      </c>
+      <c r="H6">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="3">
+        <v>44245</v>
+      </c>
+      <c r="B7">
+        <f>A7-delta_cep!A7+delta_cep!B7</f>
+        <v>1217</v>
+      </c>
+      <c r="C7">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1217.79930555556</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>5.08330555555563</v>
+      </c>
+      <c r="H7">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="3">
+        <v>44248</v>
+      </c>
+      <c r="B8">
+        <f>A8-delta_cep!A8+delta_cep!B8</f>
+        <v>1220</v>
+      </c>
+      <c r="C8">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>53</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1220.82847222222</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>2.74647222222234</v>
+      </c>
+      <c r="H8">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3">
+        <v>44368</v>
+      </c>
+      <c r="B9">
+        <f>A9-delta_cep!A9+delta_cep!B9</f>
+        <v>1340</v>
+      </c>
+      <c r="C9">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>51</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1340.99375</v>
+      </c>
+      <c r="F9" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>4.85975000000008</v>
+      </c>
+      <c r="H9">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="3">
+        <v>44395</v>
+      </c>
+      <c r="B10">
+        <f>A10-delta_cep!A10+delta_cep!B10</f>
+        <v>1367</v>
+      </c>
+      <c r="C10">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>12</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1367.925</v>
+      </c>
+      <c r="F10" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>4.96100000000001</v>
+      </c>
+      <c r="H10">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="3">
+        <v>44398</v>
+      </c>
+      <c r="B11">
+        <f>A11-delta_cep!A11+delta_cep!B11</f>
+        <v>1370</v>
+      </c>
+      <c r="C11">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>37</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>1370.90069444444</v>
+      </c>
+      <c r="F11" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>2.5706944444446</v>
+      </c>
+      <c r="H11">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="3">
+        <v>44412</v>
+      </c>
+      <c r="B12">
+        <f>A12-delta_cep!A12+delta_cep!B12</f>
+        <v>1384</v>
+      </c>
+      <c r="C12">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>1384.88680555556</v>
+      </c>
+      <c r="F12" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0.458805555555728</v>
+      </c>
+      <c r="H12">
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>